<commit_message>
Redoing analysis for quiescent behavior
</commit_message>
<xml_diff>
--- a/Tstats.xlsx
+++ b/Tstats.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="804" uniqueCount="804">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="865" uniqueCount="865">
   <si>
     <t>OriginalVariableNames</t>
   </si>
@@ -2489,6 +2489,193 @@
   </si>
   <si>
     <t>16 ± 9</t>
+  </si>
+  <si>
+    <t>OriginalVariableNames</t>
+  </si>
+  <si>
+    <t>Julian Day of Year</t>
+  </si>
+  <si>
+    <t>Recording Sessions</t>
+  </si>
+  <si>
+    <t>Unique Squirrels</t>
+  </si>
+  <si>
+    <t>Day Length (hrs)</t>
+  </si>
+  <si>
+    <t>Sleep per day (hrs)</t>
+  </si>
+  <si>
+    <t>Sleep in daylight (hrs)</t>
+  </si>
+  <si>
+    <t>Sleep in darkness (hrs)</t>
+  </si>
+  <si>
+    <t>Total sleep transitions</t>
+  </si>
+  <si>
+    <t>Sleep transitions in daylight</t>
+  </si>
+  <si>
+    <t>Sleep transitions in darkness</t>
+  </si>
+  <si>
+    <t>Winter</t>
+  </si>
+  <si>
+    <t>311-35</t>
+  </si>
+  <si>
+    <t>84</t>
+  </si>
+  <si>
+    <t>6.55 ± 0.79</t>
+  </si>
+  <si>
+    <t>13.37 ± 1.89</t>
+  </si>
+  <si>
+    <t>2.31 ± 0.86</t>
+  </si>
+  <si>
+    <t>11.07 ± 1.53</t>
+  </si>
+  <si>
+    <t>453 ± 87</t>
+  </si>
+  <si>
+    <t>94 ± 27</t>
+  </si>
+  <si>
+    <t>359 ± 78
+</t>
+  </si>
+  <si>
+    <t>Spring</t>
+  </si>
+  <si>
+    <t>36-127</t>
+  </si>
+  <si>
+    <t>88</t>
+  </si>
+  <si>
+    <t>12.44 ± 2.52</t>
+  </si>
+  <si>
+    <t>12.61 ± 2.53</t>
+  </si>
+  <si>
+    <t>3.93 ± 1.92</t>
+  </si>
+  <si>
+    <t>8.69 ± 2.07</t>
+  </si>
+  <si>
+    <t>363 ± 94</t>
+  </si>
+  <si>
+    <t>139 ± 59</t>
+  </si>
+  <si>
+    <t>223 ± 91
+</t>
+  </si>
+  <si>
+    <t>Summer</t>
+  </si>
+  <si>
+    <t>128-218</t>
+  </si>
+  <si>
+    <t>75</t>
+  </si>
+  <si>
+    <t>18.21 ± 0.81</t>
+  </si>
+  <si>
+    <t>13.30 ± 3.11</t>
+  </si>
+  <si>
+    <t>8.64 ± 2.82</t>
+  </si>
+  <si>
+    <t>4.66 ± 0.81</t>
+  </si>
+  <si>
+    <t>313 ± 56</t>
+  </si>
+  <si>
+    <t>244 ± 63</t>
+  </si>
+  <si>
+    <t>69 ± 39
+</t>
+  </si>
+  <si>
+    <t>Autumn</t>
+  </si>
+  <si>
+    <t>219-309</t>
+  </si>
+  <si>
+    <t>98</t>
+  </si>
+  <si>
+    <t>12.37 ± 2.47</t>
+  </si>
+  <si>
+    <t>10.77 ± 3.13</t>
+  </si>
+  <si>
+    <t>3.19 ± 2.60</t>
+  </si>
+  <si>
+    <t>7.58 ± 1.30</t>
+  </si>
+  <si>
+    <t>283 ± 74</t>
+  </si>
+  <si>
+    <t>122 ± 83</t>
+  </si>
+  <si>
+    <t>161 ± 68
+</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>1-366</t>
+  </si>
+  <si>
+    <t>345</t>
+  </si>
+  <si>
+    <t>12.38 ± 4.52</t>
+  </si>
+  <si>
+    <t>12.66 ± 2.86</t>
+  </si>
+  <si>
+    <t>4.55 ± 3.36</t>
+  </si>
+  <si>
+    <t>8.10 ± 2.88</t>
+  </si>
+  <si>
+    <t>361 ± 104</t>
+  </si>
+  <si>
+    <t>150 ± 84</t>
+  </si>
+  <si>
+    <t>211 ± 135</t>
   </si>
 </sst>
 </file>
@@ -2509,7 +2696,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -2533,11 +2720,12 @@
     <border/>
     <border/>
     <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -2555,6 +2743,7 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2577,67 +2766,67 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>743</v>
+        <v>804</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>754</v>
+        <v>815</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>764</v>
+        <v>825</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>774</v>
+        <v>835</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>784</v>
+        <v>845</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>794</v>
+        <v>855</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>744</v>
+        <v>805</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>755</v>
+        <v>816</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>765</v>
+        <v>826</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>775</v>
+        <v>836</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>785</v>
+        <v>846</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>795</v>
+        <v>856</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>745</v>
+        <v>806</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>756</v>
+        <v>817</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>766</v>
+        <v>827</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>776</v>
+        <v>837</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>786</v>
+        <v>847</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>796</v>
+        <v>857</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>746</v>
+        <v>807</v>
       </c>
       <c r="B4" s="0">
         <v>71</v>
@@ -2657,142 +2846,142 @@
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>747</v>
+        <v>808</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>757</v>
+        <v>818</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>767</v>
+        <v>828</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>777</v>
+        <v>838</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>787</v>
+        <v>848</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>797</v>
+        <v>858</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>748</v>
+        <v>809</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>758</v>
+        <v>819</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>768</v>
+        <v>829</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>778</v>
+        <v>839</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>788</v>
+        <v>849</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>798</v>
+        <v>859</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>749</v>
+        <v>810</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>759</v>
+        <v>820</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>769</v>
+        <v>830</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>779</v>
+        <v>840</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>789</v>
+        <v>850</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>799</v>
+        <v>860</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
-        <v>750</v>
+        <v>811</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>760</v>
+        <v>821</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>770</v>
+        <v>831</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>780</v>
+        <v>841</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>790</v>
+        <v>851</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>800</v>
+        <v>861</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0" t="s">
-        <v>751</v>
+        <v>812</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>761</v>
+        <v>822</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>771</v>
+        <v>832</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>781</v>
+        <v>842</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>791</v>
+        <v>852</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>801</v>
+        <v>862</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
-        <v>752</v>
+        <v>813</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>762</v>
+        <v>823</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>772</v>
+        <v>833</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>782</v>
+        <v>843</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>792</v>
+        <v>853</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>802</v>
+        <v>863</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0" t="s">
-        <v>753</v>
+        <v>814</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>763</v>
+        <v>824</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>773</v>
+        <v>834</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>783</v>
+        <v>844</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>793</v>
+        <v>854</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>803</v>
+        <v>864</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates to sleep-wake alg, updating figs
</commit_message>
<xml_diff>
--- a/Tstats.xlsx
+++ b/Tstats.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="865" uniqueCount="865">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1960" uniqueCount="1960">
   <si>
     <t>OriginalVariableNames</t>
   </si>
@@ -2676,6 +2676,3408 @@
   </si>
   <si>
     <t>211 ± 135</t>
+  </si>
+  <si>
+    <t>OriginalVariableNames</t>
+  </si>
+  <si>
+    <t>Julian Day of Year</t>
+  </si>
+  <si>
+    <t>Recording Sessions</t>
+  </si>
+  <si>
+    <t>Unique Squirrels</t>
+  </si>
+  <si>
+    <t>Day Length (hrs)</t>
+  </si>
+  <si>
+    <t>QB per day (hrs)</t>
+  </si>
+  <si>
+    <t>QB in daylight (hrs)</t>
+  </si>
+  <si>
+    <t>QB in daylight (%)</t>
+  </si>
+  <si>
+    <t>QB in darkness (hrs)</t>
+  </si>
+  <si>
+    <t>QB in darkness (%)</t>
+  </si>
+  <si>
+    <t>Total QB transitions</t>
+  </si>
+  <si>
+    <t>QB transitions in daylight</t>
+  </si>
+  <si>
+    <t>QB transitions per-hour daylight</t>
+  </si>
+  <si>
+    <t>QB transitions in darkness</t>
+  </si>
+  <si>
+    <t>QB transitions per-hour darkness</t>
+  </si>
+  <si>
+    <t>Winter</t>
+  </si>
+  <si>
+    <t>311-35</t>
+  </si>
+  <si>
+    <t>84</t>
+  </si>
+  <si>
+    <t>6.55 ± 0.79</t>
+  </si>
+  <si>
+    <t>13.37 ± 1.89</t>
+  </si>
+  <si>
+    <t>2.31 ± 0.86</t>
+  </si>
+  <si>
+    <t>35% ± 13%</t>
+  </si>
+  <si>
+    <t>11.07 ± 1.53</t>
+  </si>
+  <si>
+    <t>63% ± 9%</t>
+  </si>
+  <si>
+    <t>453 ± 87</t>
+  </si>
+  <si>
+    <t>94 ± 27</t>
+  </si>
+  <si>
+    <t>14 ± 4</t>
+  </si>
+  <si>
+    <t>359 ± 78
+</t>
+  </si>
+  <si>
+    <t>2058 ± 447
+</t>
+  </si>
+  <si>
+    <t>Spring</t>
+  </si>
+  <si>
+    <t>36-127</t>
+  </si>
+  <si>
+    <t>88</t>
+  </si>
+  <si>
+    <t>12.44 ± 2.52</t>
+  </si>
+  <si>
+    <t>12.61 ± 2.53</t>
+  </si>
+  <si>
+    <t>3.93 ± 1.92</t>
+  </si>
+  <si>
+    <t>32% ± 15%</t>
+  </si>
+  <si>
+    <t>8.69 ± 2.07</t>
+  </si>
+  <si>
+    <t>75% ± 18%</t>
+  </si>
+  <si>
+    <t>363 ± 94</t>
+  </si>
+  <si>
+    <t>139 ± 59</t>
+  </si>
+  <si>
+    <t>11 ± 5</t>
+  </si>
+  <si>
+    <t>223 ± 91
+</t>
+  </si>
+  <si>
+    <t>1930 ± 789
+</t>
+  </si>
+  <si>
+    <t>Summer</t>
+  </si>
+  <si>
+    <t>128-218</t>
+  </si>
+  <si>
+    <t>75</t>
+  </si>
+  <si>
+    <t>18.21 ± 0.81</t>
+  </si>
+  <si>
+    <t>13.30 ± 3.11</t>
+  </si>
+  <si>
+    <t>8.64 ± 2.82</t>
+  </si>
+  <si>
+    <t>47% ± 16%</t>
+  </si>
+  <si>
+    <t>4.66 ± 0.81</t>
+  </si>
+  <si>
+    <t>81% ± 14%</t>
+  </si>
+  <si>
+    <t>313 ± 56</t>
+  </si>
+  <si>
+    <t>244 ± 63</t>
+  </si>
+  <si>
+    <t>13 ± 3</t>
+  </si>
+  <si>
+    <t>69 ± 39
+</t>
+  </si>
+  <si>
+    <t>1188 ± 676
+</t>
+  </si>
+  <si>
+    <t>Autumn</t>
+  </si>
+  <si>
+    <t>219-309</t>
+  </si>
+  <si>
+    <t>98</t>
+  </si>
+  <si>
+    <t>12.37 ± 2.47</t>
+  </si>
+  <si>
+    <t>10.77 ± 3.13</t>
+  </si>
+  <si>
+    <t>3.19 ± 2.60</t>
+  </si>
+  <si>
+    <t>26% ± 21%</t>
+  </si>
+  <si>
+    <t>7.58 ± 1.30</t>
+  </si>
+  <si>
+    <t>65% ± 11%</t>
+  </si>
+  <si>
+    <t>283 ± 74</t>
+  </si>
+  <si>
+    <t>122 ± 83</t>
+  </si>
+  <si>
+    <t>10 ± 7</t>
+  </si>
+  <si>
+    <t>161 ± 68
+</t>
+  </si>
+  <si>
+    <t>1382 ± 584
+</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>1-366</t>
+  </si>
+  <si>
+    <t>345</t>
+  </si>
+  <si>
+    <t>12.38 ± 4.52</t>
+  </si>
+  <si>
+    <t>12.66 ± 2.86</t>
+  </si>
+  <si>
+    <t>4.55 ± 3.36</t>
+  </si>
+  <si>
+    <t>37% ± 27%</t>
+  </si>
+  <si>
+    <t>8.10 ± 2.88</t>
+  </si>
+  <si>
+    <t>70% ± 25%</t>
+  </si>
+  <si>
+    <t>361 ± 104</t>
+  </si>
+  <si>
+    <t>150 ± 84</t>
+  </si>
+  <si>
+    <t>12 ± 7</t>
+  </si>
+  <si>
+    <t>211 ± 135</t>
+  </si>
+  <si>
+    <t>1813 ± 1159
+</t>
+  </si>
+  <si>
+    <t>OriginalVariableNames</t>
+  </si>
+  <si>
+    <t>Julian Day of Year</t>
+  </si>
+  <si>
+    <t>Recording Sessions</t>
+  </si>
+  <si>
+    <t>Unique Squirrels</t>
+  </si>
+  <si>
+    <t>Day Length (hrs)</t>
+  </si>
+  <si>
+    <t>QB per day (hrs)</t>
+  </si>
+  <si>
+    <t>QB in daylight (hrs)</t>
+  </si>
+  <si>
+    <t>QB in daylight (%)</t>
+  </si>
+  <si>
+    <t>QB in darkness (hrs)</t>
+  </si>
+  <si>
+    <t>QB in darkness (%)</t>
+  </si>
+  <si>
+    <t>Total QB transitions</t>
+  </si>
+  <si>
+    <t>QB transitions in daylight</t>
+  </si>
+  <si>
+    <t>QB transitions per-hour daylight</t>
+  </si>
+  <si>
+    <t>QB transitions in darkness</t>
+  </si>
+  <si>
+    <t>QB transitions per-hour darkness</t>
+  </si>
+  <si>
+    <t>Winter</t>
+  </si>
+  <si>
+    <t>311-35</t>
+  </si>
+  <si>
+    <t>84</t>
+  </si>
+  <si>
+    <t>6.55 ± 0.79</t>
+  </si>
+  <si>
+    <t>13.37 ± 1.89</t>
+  </si>
+  <si>
+    <t>2.31 ± 0.86</t>
+  </si>
+  <si>
+    <t>35% ± 13%</t>
+  </si>
+  <si>
+    <t>11.07 ± 1.53</t>
+  </si>
+  <si>
+    <t>63% ± 9%</t>
+  </si>
+  <si>
+    <t>453 ± 87</t>
+  </si>
+  <si>
+    <t>94 ± 27</t>
+  </si>
+  <si>
+    <t>14 ± 4</t>
+  </si>
+  <si>
+    <t>359 ± 78
+</t>
+  </si>
+  <si>
+    <t>21 ± 4
+</t>
+  </si>
+  <si>
+    <t>Spring</t>
+  </si>
+  <si>
+    <t>36-127</t>
+  </si>
+  <si>
+    <t>88</t>
+  </si>
+  <si>
+    <t>12.44 ± 2.52</t>
+  </si>
+  <si>
+    <t>12.61 ± 2.53</t>
+  </si>
+  <si>
+    <t>3.93 ± 1.92</t>
+  </si>
+  <si>
+    <t>32% ± 15%</t>
+  </si>
+  <si>
+    <t>8.69 ± 2.07</t>
+  </si>
+  <si>
+    <t>75% ± 18%</t>
+  </si>
+  <si>
+    <t>363 ± 94</t>
+  </si>
+  <si>
+    <t>139 ± 59</t>
+  </si>
+  <si>
+    <t>11 ± 5</t>
+  </si>
+  <si>
+    <t>223 ± 91
+</t>
+  </si>
+  <si>
+    <t>19 ± 8
+</t>
+  </si>
+  <si>
+    <t>Summer</t>
+  </si>
+  <si>
+    <t>128-218</t>
+  </si>
+  <si>
+    <t>75</t>
+  </si>
+  <si>
+    <t>18.21 ± 0.81</t>
+  </si>
+  <si>
+    <t>13.30 ± 3.11</t>
+  </si>
+  <si>
+    <t>8.64 ± 2.82</t>
+  </si>
+  <si>
+    <t>47% ± 16%</t>
+  </si>
+  <si>
+    <t>4.66 ± 0.81</t>
+  </si>
+  <si>
+    <t>81% ± 14%</t>
+  </si>
+  <si>
+    <t>313 ± 56</t>
+  </si>
+  <si>
+    <t>244 ± 63</t>
+  </si>
+  <si>
+    <t>13 ± 3</t>
+  </si>
+  <si>
+    <t>69 ± 39
+</t>
+  </si>
+  <si>
+    <t>12 ± 7
+</t>
+  </si>
+  <si>
+    <t>Autumn</t>
+  </si>
+  <si>
+    <t>219-309</t>
+  </si>
+  <si>
+    <t>98</t>
+  </si>
+  <si>
+    <t>12.37 ± 2.47</t>
+  </si>
+  <si>
+    <t>10.77 ± 3.13</t>
+  </si>
+  <si>
+    <t>3.19 ± 2.60</t>
+  </si>
+  <si>
+    <t>26% ± 21%</t>
+  </si>
+  <si>
+    <t>7.58 ± 1.30</t>
+  </si>
+  <si>
+    <t>65% ± 11%</t>
+  </si>
+  <si>
+    <t>283 ± 74</t>
+  </si>
+  <si>
+    <t>122 ± 83</t>
+  </si>
+  <si>
+    <t>10 ± 7</t>
+  </si>
+  <si>
+    <t>161 ± 68
+</t>
+  </si>
+  <si>
+    <t>14 ± 6
+</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>1-366</t>
+  </si>
+  <si>
+    <t>345</t>
+  </si>
+  <si>
+    <t>12.38 ± 4.52</t>
+  </si>
+  <si>
+    <t>12.66 ± 2.86</t>
+  </si>
+  <si>
+    <t>4.55 ± 3.36</t>
+  </si>
+  <si>
+    <t>37% ± 27%</t>
+  </si>
+  <si>
+    <t>8.10 ± 2.88</t>
+  </si>
+  <si>
+    <t>70% ± 25%</t>
+  </si>
+  <si>
+    <t>361 ± 104</t>
+  </si>
+  <si>
+    <t>150 ± 84</t>
+  </si>
+  <si>
+    <t>12 ± 7</t>
+  </si>
+  <si>
+    <t>211 ± 135</t>
+  </si>
+  <si>
+    <t>18 ± 12
+</t>
+  </si>
+  <si>
+    <t>OriginalVariableNames</t>
+  </si>
+  <si>
+    <t>Julian Day of Year</t>
+  </si>
+  <si>
+    <t>Recording Sessions</t>
+  </si>
+  <si>
+    <t>Unique Squirrels</t>
+  </si>
+  <si>
+    <t>Day Length (hrs)</t>
+  </si>
+  <si>
+    <t>QB per day (hrs)</t>
+  </si>
+  <si>
+    <t>QB in daylight (hrs)</t>
+  </si>
+  <si>
+    <t>QB in daylight (%)</t>
+  </si>
+  <si>
+    <t>QB in darkness (hrs)</t>
+  </si>
+  <si>
+    <t>QB in darkness (%)</t>
+  </si>
+  <si>
+    <t>Total QB transitions</t>
+  </si>
+  <si>
+    <t>QB transitions in daylight</t>
+  </si>
+  <si>
+    <t>QB transitions per-hour daylight</t>
+  </si>
+  <si>
+    <t>QB transitions in darkness</t>
+  </si>
+  <si>
+    <t>QB transitions per-hour darkness</t>
+  </si>
+  <si>
+    <t>Winter</t>
+  </si>
+  <si>
+    <t>311-35</t>
+  </si>
+  <si>
+    <t>84</t>
+  </si>
+  <si>
+    <t>6.55 ± 0.79</t>
+  </si>
+  <si>
+    <t>20.07 ± 1.30</t>
+  </si>
+  <si>
+    <t>4.16 ± 0.97</t>
+  </si>
+  <si>
+    <t>63% ± 15%</t>
+  </si>
+  <si>
+    <t>15.91 ± 1.05</t>
+  </si>
+  <si>
+    <t>91% ± 6%</t>
+  </si>
+  <si>
+    <t>194 ± 38</t>
+  </si>
+  <si>
+    <t>88 ± 28</t>
+  </si>
+  <si>
+    <t>13 ± 4</t>
+  </si>
+  <si>
+    <t>106 ± 32
+</t>
+  </si>
+  <si>
+    <t>6 ± 2
+</t>
+  </si>
+  <si>
+    <t>Spring</t>
+  </si>
+  <si>
+    <t>36-127</t>
+  </si>
+  <si>
+    <t>88</t>
+  </si>
+  <si>
+    <t>12.44 ± 2.52</t>
+  </si>
+  <si>
+    <t>18.16 ± 2.38</t>
+  </si>
+  <si>
+    <t>6.89 ± 1.88</t>
+  </si>
+  <si>
+    <t>55% ± 15%</t>
+  </si>
+  <si>
+    <t>11.27 ± 2.44</t>
+  </si>
+  <si>
+    <t>98% ± 21%</t>
+  </si>
+  <si>
+    <t>249 ± 47</t>
+  </si>
+  <si>
+    <t>184 ± 49</t>
+  </si>
+  <si>
+    <t>15 ± 4</t>
+  </si>
+  <si>
+    <t>65 ± 28
+</t>
+  </si>
+  <si>
+    <t>6 ± 2
+</t>
+  </si>
+  <si>
+    <t>Summer</t>
+  </si>
+  <si>
+    <t>128-218</t>
+  </si>
+  <si>
+    <t>75</t>
+  </si>
+  <si>
+    <t>18.21 ± 0.81</t>
+  </si>
+  <si>
+    <t>16.70 ± 1.81</t>
+  </si>
+  <si>
+    <t>11.46 ± 2.03</t>
+  </si>
+  <si>
+    <t>63% ± 11%</t>
+  </si>
+  <si>
+    <t>5.24 ± 0.71</t>
+  </si>
+  <si>
+    <t>90% ± 12%</t>
+  </si>
+  <si>
+    <t>314 ± 49</t>
+  </si>
+  <si>
+    <t>284 ± 48</t>
+  </si>
+  <si>
+    <t>16 ± 3</t>
+  </si>
+  <si>
+    <t>30 ± 16
+</t>
+  </si>
+  <si>
+    <t>5 ± 3
+</t>
+  </si>
+  <si>
+    <t>Autumn</t>
+  </si>
+  <si>
+    <t>219-309</t>
+  </si>
+  <si>
+    <t>98</t>
+  </si>
+  <si>
+    <t>12.37 ± 2.47</t>
+  </si>
+  <si>
+    <t>14.10 ± 2.12</t>
+  </si>
+  <si>
+    <t>4.87 ± 2.24</t>
+  </si>
+  <si>
+    <t>39% ± 18%</t>
+  </si>
+  <si>
+    <t>9.22 ± 1.08</t>
+  </si>
+  <si>
+    <t>79% ± 9%</t>
+  </si>
+  <si>
+    <t>258 ± 56</t>
+  </si>
+  <si>
+    <t>193 ± 49</t>
+  </si>
+  <si>
+    <t>16 ± 4</t>
+  </si>
+  <si>
+    <t>66 ± 21
+</t>
+  </si>
+  <si>
+    <t>6 ± 2
+</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>1-366</t>
+  </si>
+  <si>
+    <t>345</t>
+  </si>
+  <si>
+    <t>12.38 ± 4.52</t>
+  </si>
+  <si>
+    <t>17.50 ± 2.88</t>
+  </si>
+  <si>
+    <t>6.85 ± 3.50</t>
+  </si>
+  <si>
+    <t>55% ± 28%</t>
+  </si>
+  <si>
+    <t>10.66 ± 4.40</t>
+  </si>
+  <si>
+    <t>92% ± 38%</t>
+  </si>
+  <si>
+    <t>251 ± 66</t>
+  </si>
+  <si>
+    <t>183 ± 87</t>
+  </si>
+  <si>
+    <t>15 ± 7</t>
+  </si>
+  <si>
+    <t>69 ± 39</t>
+  </si>
+  <si>
+    <t>6 ± 3
+</t>
+  </si>
+  <si>
+    <t>OriginalVariableNames</t>
+  </si>
+  <si>
+    <t>Julian Day of Year</t>
+  </si>
+  <si>
+    <t>Recording Sessions</t>
+  </si>
+  <si>
+    <t>Unique Squirrels</t>
+  </si>
+  <si>
+    <t>Day Length (hrs)</t>
+  </si>
+  <si>
+    <t>QB per day (hrs)</t>
+  </si>
+  <si>
+    <t>QB in daylight (hrs)</t>
+  </si>
+  <si>
+    <t>QB in daylight (%)</t>
+  </si>
+  <si>
+    <t>QB in darkness (hrs)</t>
+  </si>
+  <si>
+    <t>QB in darkness (%)</t>
+  </si>
+  <si>
+    <t>Total QB transitions</t>
+  </si>
+  <si>
+    <t>QB transitions in daylight</t>
+  </si>
+  <si>
+    <t>QB transitions per-hour daylight</t>
+  </si>
+  <si>
+    <t>QB transitions in darkness</t>
+  </si>
+  <si>
+    <t>QB transitions per-hour darkness</t>
+  </si>
+  <si>
+    <t>Winter</t>
+  </si>
+  <si>
+    <t>311-35</t>
+  </si>
+  <si>
+    <t>84</t>
+  </si>
+  <si>
+    <t>6.55 ± 0.79</t>
+  </si>
+  <si>
+    <t>13.47 ± 2.14</t>
+  </si>
+  <si>
+    <t>2.33 ± 0.90</t>
+  </si>
+  <si>
+    <t>36% ± 14%</t>
+  </si>
+  <si>
+    <t>11.14 ± 1.72</t>
+  </si>
+  <si>
+    <t>64% ± 10%</t>
+  </si>
+  <si>
+    <t>447 ± 92</t>
+  </si>
+  <si>
+    <t>93 ± 27</t>
+  </si>
+  <si>
+    <t>14 ± 4</t>
+  </si>
+  <si>
+    <t>354 ± 82
+</t>
+  </si>
+  <si>
+    <t>20 ± 5
+</t>
+  </si>
+  <si>
+    <t>Spring</t>
+  </si>
+  <si>
+    <t>36-127</t>
+  </si>
+  <si>
+    <t>88</t>
+  </si>
+  <si>
+    <t>12.44 ± 2.52</t>
+  </si>
+  <si>
+    <t>13.55 ± 3.05</t>
+  </si>
+  <si>
+    <t>4.26 ± 1.55</t>
+  </si>
+  <si>
+    <t>34% ± 12%</t>
+  </si>
+  <si>
+    <t>9.28 ± 2.71</t>
+  </si>
+  <si>
+    <t>80% ± 23%</t>
+  </si>
+  <si>
+    <t>321 ± 124</t>
+  </si>
+  <si>
+    <t>145 ± 46</t>
+  </si>
+  <si>
+    <t>12 ± 4</t>
+  </si>
+  <si>
+    <t>176 ± 105
+</t>
+  </si>
+  <si>
+    <t>15 ± 9
+</t>
+  </si>
+  <si>
+    <t>Summer</t>
+  </si>
+  <si>
+    <t>128-218</t>
+  </si>
+  <si>
+    <t>75</t>
+  </si>
+  <si>
+    <t>18.21 ± 0.81</t>
+  </si>
+  <si>
+    <t>11.21 ± 2.20</t>
+  </si>
+  <si>
+    <t>6.92 ± 1.90</t>
+  </si>
+  <si>
+    <t>38% ± 10%</t>
+  </si>
+  <si>
+    <t>4.29 ± 0.97</t>
+  </si>
+  <si>
+    <t>74% ± 17%</t>
+  </si>
+  <si>
+    <t>313 ± 87</t>
+  </si>
+  <si>
+    <t>227 ± 62</t>
+  </si>
+  <si>
+    <t>12 ± 3</t>
+  </si>
+  <si>
+    <t>85 ± 41
+</t>
+  </si>
+  <si>
+    <t>15 ± 7
+</t>
+  </si>
+  <si>
+    <t>Autumn</t>
+  </si>
+  <si>
+    <t>219-309</t>
+  </si>
+  <si>
+    <t>98</t>
+  </si>
+  <si>
+    <t>12.37 ± 2.47</t>
+  </si>
+  <si>
+    <t>10.06 ± 2.25</t>
+  </si>
+  <si>
+    <t>2.57 ± 1.82</t>
+  </si>
+  <si>
+    <t>21% ± 15%</t>
+  </si>
+  <si>
+    <t>7.49 ± 1.59</t>
+  </si>
+  <si>
+    <t>64% ± 14%</t>
+  </si>
+  <si>
+    <t>271 ± 89</t>
+  </si>
+  <si>
+    <t>110 ± 55</t>
+  </si>
+  <si>
+    <t>9 ± 4</t>
+  </si>
+  <si>
+    <t>161 ± 61
+</t>
+  </si>
+  <si>
+    <t>14 ± 5
+</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>1-366</t>
+  </si>
+  <si>
+    <t>345</t>
+  </si>
+  <si>
+    <t>12.38 ± 4.52</t>
+  </si>
+  <si>
+    <t>12.14 ± 2.78</t>
+  </si>
+  <si>
+    <t>4.02 ± 2.47</t>
+  </si>
+  <si>
+    <t>32% ± 20%</t>
+  </si>
+  <si>
+    <t>8.12 ± 3.23</t>
+  </si>
+  <si>
+    <t>70% ± 28%</t>
+  </si>
+  <si>
+    <t>348 ± 120</t>
+  </si>
+  <si>
+    <t>144 ± 73</t>
+  </si>
+  <si>
+    <t>12 ± 6</t>
+  </si>
+  <si>
+    <t>205 ± 131</t>
+  </si>
+  <si>
+    <t>18 ± 11
+</t>
+  </si>
+  <si>
+    <t>OriginalVariableNames</t>
+  </si>
+  <si>
+    <t>Julian Day of Year</t>
+  </si>
+  <si>
+    <t>Recording Sessions</t>
+  </si>
+  <si>
+    <t>Unique Squirrels</t>
+  </si>
+  <si>
+    <t>Day Length (hrs)</t>
+  </si>
+  <si>
+    <t>QB per day (hrs)</t>
+  </si>
+  <si>
+    <t>QB in daylight (hrs)</t>
+  </si>
+  <si>
+    <t>QB in daylight (%)</t>
+  </si>
+  <si>
+    <t>QB in darkness (hrs)</t>
+  </si>
+  <si>
+    <t>QB in darkness (%)</t>
+  </si>
+  <si>
+    <t>Total QB transitions</t>
+  </si>
+  <si>
+    <t>QB transitions in daylight</t>
+  </si>
+  <si>
+    <t>QB transitions per-hour daylight</t>
+  </si>
+  <si>
+    <t>QB transitions in darkness</t>
+  </si>
+  <si>
+    <t>QB transitions per-hour darkness</t>
+  </si>
+  <si>
+    <t>Winter</t>
+  </si>
+  <si>
+    <t>311-35</t>
+  </si>
+  <si>
+    <t>84</t>
+  </si>
+  <si>
+    <t>6.55 ± 0.79</t>
+  </si>
+  <si>
+    <t>19.24 ± 1.44</t>
+  </si>
+  <si>
+    <t>3.82 ± 0.96</t>
+  </si>
+  <si>
+    <t>58% ± 15%</t>
+  </si>
+  <si>
+    <t>15.42 ± 1.19</t>
+  </si>
+  <si>
+    <t>88% ± 7%</t>
+  </si>
+  <si>
+    <t>210 ± 47</t>
+  </si>
+  <si>
+    <t>85 ± 25</t>
+  </si>
+  <si>
+    <t>13 ± 4</t>
+  </si>
+  <si>
+    <t>125 ± 46
+</t>
+  </si>
+  <si>
+    <t>7 ± 3
+</t>
+  </si>
+  <si>
+    <t>Spring</t>
+  </si>
+  <si>
+    <t>36-127</t>
+  </si>
+  <si>
+    <t>88</t>
+  </si>
+  <si>
+    <t>12.44 ± 2.52</t>
+  </si>
+  <si>
+    <t>17.52 ± 2.50</t>
+  </si>
+  <si>
+    <t>6.37 ± 1.98</t>
+  </si>
+  <si>
+    <t>51% ± 16%</t>
+  </si>
+  <si>
+    <t>11.15 ± 2.41</t>
+  </si>
+  <si>
+    <t>96% ± 21%</t>
+  </si>
+  <si>
+    <t>238 ± 46</t>
+  </si>
+  <si>
+    <t>167 ± 48</t>
+  </si>
+  <si>
+    <t>13 ± 4</t>
+  </si>
+  <si>
+    <t>71 ± 30
+</t>
+  </si>
+  <si>
+    <t>6 ± 3
+</t>
+  </si>
+  <si>
+    <t>Summer</t>
+  </si>
+  <si>
+    <t>128-218</t>
+  </si>
+  <si>
+    <t>75</t>
+  </si>
+  <si>
+    <t>18.21 ± 0.81</t>
+  </si>
+  <si>
+    <t>15.93 ± 1.91</t>
+  </si>
+  <si>
+    <t>10.75 ± 2.10</t>
+  </si>
+  <si>
+    <t>59% ± 12%</t>
+  </si>
+  <si>
+    <t>5.18 ± 0.73</t>
+  </si>
+  <si>
+    <t>90% ± 13%</t>
+  </si>
+  <si>
+    <t>305 ± 50</t>
+  </si>
+  <si>
+    <t>272 ± 48</t>
+  </si>
+  <si>
+    <t>15 ± 3</t>
+  </si>
+  <si>
+    <t>32 ± 16
+</t>
+  </si>
+  <si>
+    <t>6 ± 3
+</t>
+  </si>
+  <si>
+    <t>Autumn</t>
+  </si>
+  <si>
+    <t>219-309</t>
+  </si>
+  <si>
+    <t>98</t>
+  </si>
+  <si>
+    <t>12.37 ± 2.47</t>
+  </si>
+  <si>
+    <t>13.78 ± 2.19</t>
+  </si>
+  <si>
+    <t>4.63 ± 2.31</t>
+  </si>
+  <si>
+    <t>37% ± 19%</t>
+  </si>
+  <si>
+    <t>9.15 ± 1.07</t>
+  </si>
+  <si>
+    <t>79% ± 9%</t>
+  </si>
+  <si>
+    <t>248 ± 58</t>
+  </si>
+  <si>
+    <t>180 ± 52</t>
+  </si>
+  <si>
+    <t>15 ± 4</t>
+  </si>
+  <si>
+    <t>68 ± 22
+</t>
+  </si>
+  <si>
+    <t>6 ± 2
+</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>1-366</t>
+  </si>
+  <si>
+    <t>345</t>
+  </si>
+  <si>
+    <t>12.38 ± 4.52</t>
+  </si>
+  <si>
+    <t>16.84 ± 2.83</t>
+  </si>
+  <si>
+    <t>6.39 ± 3.38</t>
+  </si>
+  <si>
+    <t>52% ± 27%</t>
+  </si>
+  <si>
+    <t>10.45 ± 4.24</t>
+  </si>
+  <si>
+    <t>90% ± 37%</t>
+  </si>
+  <si>
+    <t>250 ± 62</t>
+  </si>
+  <si>
+    <t>173 ± 84</t>
+  </si>
+  <si>
+    <t>14 ± 7</t>
+  </si>
+  <si>
+    <t>77 ± 48</t>
+  </si>
+  <si>
+    <t>7 ± 4
+</t>
+  </si>
+  <si>
+    <t>OriginalVariableNames</t>
+  </si>
+  <si>
+    <t>Julian Day of Year</t>
+  </si>
+  <si>
+    <t>Recording Sessions</t>
+  </si>
+  <si>
+    <t>Unique Squirrels</t>
+  </si>
+  <si>
+    <t>Day Length (hrs)</t>
+  </si>
+  <si>
+    <t>QB per day (hrs)</t>
+  </si>
+  <si>
+    <t>QB in daylight (hrs)</t>
+  </si>
+  <si>
+    <t>QB in daylight (%)</t>
+  </si>
+  <si>
+    <t>QB in darkness (hrs)</t>
+  </si>
+  <si>
+    <t>QB in darkness (%)</t>
+  </si>
+  <si>
+    <t>Total QB transitions</t>
+  </si>
+  <si>
+    <t>QB transitions in daylight</t>
+  </si>
+  <si>
+    <t>QB transitions per-hour daylight</t>
+  </si>
+  <si>
+    <t>QB transitions in darkness</t>
+  </si>
+  <si>
+    <t>QB transitions per-hour darkness</t>
+  </si>
+  <si>
+    <t>Winter</t>
+  </si>
+  <si>
+    <t>311-35</t>
+  </si>
+  <si>
+    <t>84</t>
+  </si>
+  <si>
+    <t>6.55 ± 0.79</t>
+  </si>
+  <si>
+    <t>19.24 ± 1.44</t>
+  </si>
+  <si>
+    <t>3.82 ± 0.96</t>
+  </si>
+  <si>
+    <t>58% ± 15%</t>
+  </si>
+  <si>
+    <t>15.42 ± 1.19</t>
+  </si>
+  <si>
+    <t>88% ± 7%</t>
+  </si>
+  <si>
+    <t>210 ± 47</t>
+  </si>
+  <si>
+    <t>85 ± 25</t>
+  </si>
+  <si>
+    <t>13 ± 4</t>
+  </si>
+  <si>
+    <t>125 ± 46
+</t>
+  </si>
+  <si>
+    <t>7 ± 3
+</t>
+  </si>
+  <si>
+    <t>Spring</t>
+  </si>
+  <si>
+    <t>36-127</t>
+  </si>
+  <si>
+    <t>88</t>
+  </si>
+  <si>
+    <t>12.44 ± 2.52</t>
+  </si>
+  <si>
+    <t>17.52 ± 2.50</t>
+  </si>
+  <si>
+    <t>6.37 ± 1.98</t>
+  </si>
+  <si>
+    <t>51% ± 16%</t>
+  </si>
+  <si>
+    <t>11.15 ± 2.41</t>
+  </si>
+  <si>
+    <t>96% ± 21%</t>
+  </si>
+  <si>
+    <t>238 ± 46</t>
+  </si>
+  <si>
+    <t>167 ± 48</t>
+  </si>
+  <si>
+    <t>13 ± 4</t>
+  </si>
+  <si>
+    <t>71 ± 30
+</t>
+  </si>
+  <si>
+    <t>6 ± 3
+</t>
+  </si>
+  <si>
+    <t>Summer</t>
+  </si>
+  <si>
+    <t>128-218</t>
+  </si>
+  <si>
+    <t>75</t>
+  </si>
+  <si>
+    <t>18.21 ± 0.81</t>
+  </si>
+  <si>
+    <t>15.93 ± 1.91</t>
+  </si>
+  <si>
+    <t>10.75 ± 2.10</t>
+  </si>
+  <si>
+    <t>59% ± 12%</t>
+  </si>
+  <si>
+    <t>5.18 ± 0.73</t>
+  </si>
+  <si>
+    <t>90% ± 13%</t>
+  </si>
+  <si>
+    <t>305 ± 50</t>
+  </si>
+  <si>
+    <t>272 ± 48</t>
+  </si>
+  <si>
+    <t>15 ± 3</t>
+  </si>
+  <si>
+    <t>32 ± 16
+</t>
+  </si>
+  <si>
+    <t>6 ± 3
+</t>
+  </si>
+  <si>
+    <t>Autumn</t>
+  </si>
+  <si>
+    <t>219-309</t>
+  </si>
+  <si>
+    <t>98</t>
+  </si>
+  <si>
+    <t>12.37 ± 2.47</t>
+  </si>
+  <si>
+    <t>13.78 ± 2.19</t>
+  </si>
+  <si>
+    <t>4.63 ± 2.31</t>
+  </si>
+  <si>
+    <t>37% ± 19%</t>
+  </si>
+  <si>
+    <t>9.15 ± 1.07</t>
+  </si>
+  <si>
+    <t>79% ± 9%</t>
+  </si>
+  <si>
+    <t>248 ± 58</t>
+  </si>
+  <si>
+    <t>180 ± 52</t>
+  </si>
+  <si>
+    <t>15 ± 4</t>
+  </si>
+  <si>
+    <t>68 ± 22
+</t>
+  </si>
+  <si>
+    <t>6 ± 2
+</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>1-366</t>
+  </si>
+  <si>
+    <t>345</t>
+  </si>
+  <si>
+    <t>12.38 ± 4.52</t>
+  </si>
+  <si>
+    <t>16.84 ± 2.83</t>
+  </si>
+  <si>
+    <t>6.39 ± 3.38</t>
+  </si>
+  <si>
+    <t>52% ± 27%</t>
+  </si>
+  <si>
+    <t>10.45 ± 4.24</t>
+  </si>
+  <si>
+    <t>90% ± 37%</t>
+  </si>
+  <si>
+    <t>250 ± 62</t>
+  </si>
+  <si>
+    <t>173 ± 84</t>
+  </si>
+  <si>
+    <t>14 ± 7</t>
+  </si>
+  <si>
+    <t>77 ± 48</t>
+  </si>
+  <si>
+    <t>7 ± 4
+</t>
+  </si>
+  <si>
+    <t>OriginalVariableNames</t>
+  </si>
+  <si>
+    <t>Julian Day of Year</t>
+  </si>
+  <si>
+    <t>Recording Sessions</t>
+  </si>
+  <si>
+    <t>Unique Squirrels</t>
+  </si>
+  <si>
+    <t>Day Length (hrs)</t>
+  </si>
+  <si>
+    <t>QB per day (hrs)</t>
+  </si>
+  <si>
+    <t>QB in daylight (hrs)</t>
+  </si>
+  <si>
+    <t>QB in daylight (%)</t>
+  </si>
+  <si>
+    <t>QB in darkness (hrs)</t>
+  </si>
+  <si>
+    <t>QB in darkness (%)</t>
+  </si>
+  <si>
+    <t>Total QB transitions</t>
+  </si>
+  <si>
+    <t>QB transitions in daylight</t>
+  </si>
+  <si>
+    <t>QB transitions per-hour daylight</t>
+  </si>
+  <si>
+    <t>QB transitions in darkness</t>
+  </si>
+  <si>
+    <t>QB transitions per-hour darkness</t>
+  </si>
+  <si>
+    <t>Winter</t>
+  </si>
+  <si>
+    <t>311-35</t>
+  </si>
+  <si>
+    <t>84</t>
+  </si>
+  <si>
+    <t>6.55 ± 0.79</t>
+  </si>
+  <si>
+    <t>19.41 ± 1.24</t>
+  </si>
+  <si>
+    <t>3.82 ± 0.94</t>
+  </si>
+  <si>
+    <t>58% ± 14%</t>
+  </si>
+  <si>
+    <t>15.59 ± 1.05</t>
+  </si>
+  <si>
+    <t>89% ± 6%</t>
+  </si>
+  <si>
+    <t>199 ± 36</t>
+  </si>
+  <si>
+    <t>82 ± 25</t>
+  </si>
+  <si>
+    <t>12 ± 4</t>
+  </si>
+  <si>
+    <t>117 ± 30
+</t>
+  </si>
+  <si>
+    <t>7 ± 2
+</t>
+  </si>
+  <si>
+    <t>Spring</t>
+  </si>
+  <si>
+    <t>36-127</t>
+  </si>
+  <si>
+    <t>88</t>
+  </si>
+  <si>
+    <t>12.44 ± 2.52</t>
+  </si>
+  <si>
+    <t>16.76 ± 2.27</t>
+  </si>
+  <si>
+    <t>5.78 ± 1.83</t>
+  </si>
+  <si>
+    <t>46% ± 15%</t>
+  </si>
+  <si>
+    <t>10.98 ± 2.39</t>
+  </si>
+  <si>
+    <t>95% ± 21%</t>
+  </si>
+  <si>
+    <t>230 ± 49</t>
+  </si>
+  <si>
+    <t>148 ± 48</t>
+  </si>
+  <si>
+    <t>12 ± 4</t>
+  </si>
+  <si>
+    <t>82 ± 28
+</t>
+  </si>
+  <si>
+    <t>7 ± 2
+</t>
+  </si>
+  <si>
+    <t>Summer</t>
+  </si>
+  <si>
+    <t>128-218</t>
+  </si>
+  <si>
+    <t>75</t>
+  </si>
+  <si>
+    <t>18.21 ± 0.81</t>
+  </si>
+  <si>
+    <t>14.14 ± 2.13</t>
+  </si>
+  <si>
+    <t>9.15 ± 2.25</t>
+  </si>
+  <si>
+    <t>50% ± 12%</t>
+  </si>
+  <si>
+    <t>4.99 ± 0.72</t>
+  </si>
+  <si>
+    <t>86% ± 13%</t>
+  </si>
+  <si>
+    <t>279 ± 54</t>
+  </si>
+  <si>
+    <t>231 ± 50</t>
+  </si>
+  <si>
+    <t>13 ± 3</t>
+  </si>
+  <si>
+    <t>48 ± 21
+</t>
+  </si>
+  <si>
+    <t>8 ± 4
+</t>
+  </si>
+  <si>
+    <t>Autumn</t>
+  </si>
+  <si>
+    <t>219-309</t>
+  </si>
+  <si>
+    <t>98</t>
+  </si>
+  <si>
+    <t>12.37 ± 2.47</t>
+  </si>
+  <si>
+    <t>13.08 ± 2.42</t>
+  </si>
+  <si>
+    <t>4.12 ± 2.33</t>
+  </si>
+  <si>
+    <t>33% ± 19%</t>
+  </si>
+  <si>
+    <t>8.96 ± 1.18</t>
+  </si>
+  <si>
+    <t>77% ± 10%</t>
+  </si>
+  <si>
+    <t>234 ± 61</t>
+  </si>
+  <si>
+    <t>155 ± 49</t>
+  </si>
+  <si>
+    <t>13 ± 4</t>
+  </si>
+  <si>
+    <t>79 ± 33
+</t>
+  </si>
+  <si>
+    <t>7 ± 3
+</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>1-366</t>
+  </si>
+  <si>
+    <t>345</t>
+  </si>
+  <si>
+    <t>12.38 ± 4.52</t>
+  </si>
+  <si>
+    <t>16.10 ± 3.25</t>
+  </si>
+  <si>
+    <t>5.73 ± 2.90</t>
+  </si>
+  <si>
+    <t>46% ± 23%</t>
+  </si>
+  <si>
+    <t>10.37 ± 4.37</t>
+  </si>
+  <si>
+    <t>89% ± 38%</t>
+  </si>
+  <si>
+    <t>234 ± 59</t>
+  </si>
+  <si>
+    <t>151 ± 72</t>
+  </si>
+  <si>
+    <t>12 ± 6</t>
+  </si>
+  <si>
+    <t>83 ± 39</t>
+  </si>
+  <si>
+    <t>7 ± 3
+</t>
+  </si>
+  <si>
+    <t>OriginalVariableNames</t>
+  </si>
+  <si>
+    <t>Julian Day of Year</t>
+  </si>
+  <si>
+    <t>Recording Sessions</t>
+  </si>
+  <si>
+    <t>Unique Squirrels</t>
+  </si>
+  <si>
+    <t>Day Length (hrs)</t>
+  </si>
+  <si>
+    <t>QB per day (hrs)</t>
+  </si>
+  <si>
+    <t>QB in daylight (hrs)</t>
+  </si>
+  <si>
+    <t>QB in daylight (%)</t>
+  </si>
+  <si>
+    <t>QB in darkness (hrs)</t>
+  </si>
+  <si>
+    <t>QB in darkness (%)</t>
+  </si>
+  <si>
+    <t>Total QB transitions</t>
+  </si>
+  <si>
+    <t>QB transitions in daylight</t>
+  </si>
+  <si>
+    <t>QB transitions per-hour daylight</t>
+  </si>
+  <si>
+    <t>QB transitions in darkness</t>
+  </si>
+  <si>
+    <t>QB transitions per-hour darkness</t>
+  </si>
+  <si>
+    <t>Winter</t>
+  </si>
+  <si>
+    <t>311-35</t>
+  </si>
+  <si>
+    <t>84</t>
+  </si>
+  <si>
+    <t>6.55 ± 0.79</t>
+  </si>
+  <si>
+    <t>19.81 ± 1.17</t>
+  </si>
+  <si>
+    <t>4.02 ± 0.90</t>
+  </si>
+  <si>
+    <t>61% ± 14%</t>
+  </si>
+  <si>
+    <t>15.79 ± 1.04</t>
+  </si>
+  <si>
+    <t>91% ± 6%</t>
+  </si>
+  <si>
+    <t>195 ± 37</t>
+  </si>
+  <si>
+    <t>87 ± 28</t>
+  </si>
+  <si>
+    <t>13 ± 4</t>
+  </si>
+  <si>
+    <t>108 ± 29
+</t>
+  </si>
+  <si>
+    <t>6 ± 2
+</t>
+  </si>
+  <si>
+    <t>Spring</t>
+  </si>
+  <si>
+    <t>36-127</t>
+  </si>
+  <si>
+    <t>88</t>
+  </si>
+  <si>
+    <t>12.44 ± 2.52</t>
+  </si>
+  <si>
+    <t>17.70 ± 2.28</t>
+  </si>
+  <si>
+    <t>6.50 ± 1.87</t>
+  </si>
+  <si>
+    <t>52% ± 15%</t>
+  </si>
+  <si>
+    <t>11.20 ± 2.40</t>
+  </si>
+  <si>
+    <t>97% ± 21%</t>
+  </si>
+  <si>
+    <t>244 ± 45</t>
+  </si>
+  <si>
+    <t>176 ± 47</t>
+  </si>
+  <si>
+    <t>14 ± 4</t>
+  </si>
+  <si>
+    <t>68 ± 27
+</t>
+  </si>
+  <si>
+    <t>6 ± 2
+</t>
+  </si>
+  <si>
+    <t>Summer</t>
+  </si>
+  <si>
+    <t>128-218</t>
+  </si>
+  <si>
+    <t>75</t>
+  </si>
+  <si>
+    <t>18.21 ± 0.81</t>
+  </si>
+  <si>
+    <t>14.50 ± 2.00</t>
+  </si>
+  <si>
+    <t>9.45 ± 2.10</t>
+  </si>
+  <si>
+    <t>52% ± 12%</t>
+  </si>
+  <si>
+    <t>5.05 ± 0.75</t>
+  </si>
+  <si>
+    <t>87% ± 13%</t>
+  </si>
+  <si>
+    <t>279 ± 49</t>
+  </si>
+  <si>
+    <t>238 ± 44</t>
+  </si>
+  <si>
+    <t>13 ± 2</t>
+  </si>
+  <si>
+    <t>41 ± 18
+</t>
+  </si>
+  <si>
+    <t>7 ± 3
+</t>
+  </si>
+  <si>
+    <t>Autumn</t>
+  </si>
+  <si>
+    <t>219-309</t>
+  </si>
+  <si>
+    <t>98</t>
+  </si>
+  <si>
+    <t>12.37 ± 2.47</t>
+  </si>
+  <si>
+    <t>14.26 ± 1.73</t>
+  </si>
+  <si>
+    <t>5.01 ± 1.81</t>
+  </si>
+  <si>
+    <t>41% ± 15%</t>
+  </si>
+  <si>
+    <t>9.25 ± 1.14</t>
+  </si>
+  <si>
+    <t>80% ± 10%</t>
+  </si>
+  <si>
+    <t>273 ± 57</t>
+  </si>
+  <si>
+    <t>206 ± 48</t>
+  </si>
+  <si>
+    <t>17 ± 4</t>
+  </si>
+  <si>
+    <t>66 ± 23
+</t>
+  </si>
+  <si>
+    <t>6 ± 2
+</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>1-366</t>
+  </si>
+  <si>
+    <t>345</t>
+  </si>
+  <si>
+    <t>12.38 ± 4.52</t>
+  </si>
+  <si>
+    <t>16.76 ± 3.01</t>
+  </si>
+  <si>
+    <t>6.20 ± 2.76</t>
+  </si>
+  <si>
+    <t>50% ± 22%</t>
+  </si>
+  <si>
+    <t>10.56 ± 4.41</t>
+  </si>
+  <si>
+    <t>91% ± 38%</t>
+  </si>
+  <si>
+    <t>244 ± 59</t>
+  </si>
+  <si>
+    <t>171 ± 74</t>
+  </si>
+  <si>
+    <t>14 ± 6</t>
+  </si>
+  <si>
+    <t>73 ± 36</t>
+  </si>
+  <si>
+    <t>6 ± 3
+</t>
+  </si>
+  <si>
+    <t>OriginalVariableNames</t>
+  </si>
+  <si>
+    <t>Julian Day of Year</t>
+  </si>
+  <si>
+    <t>Recording Sessions</t>
+  </si>
+  <si>
+    <t>Unique Squirrels</t>
+  </si>
+  <si>
+    <t>Day Length (hrs)</t>
+  </si>
+  <si>
+    <t>QB per day (hrs)</t>
+  </si>
+  <si>
+    <t>QB in daylight (hrs)</t>
+  </si>
+  <si>
+    <t>QB in daylight (%)</t>
+  </si>
+  <si>
+    <t>QB in darkness (hrs)</t>
+  </si>
+  <si>
+    <t>QB in darkness (%)</t>
+  </si>
+  <si>
+    <t>Total QB transitions</t>
+  </si>
+  <si>
+    <t>QB transitions in daylight</t>
+  </si>
+  <si>
+    <t>QB transitions per-hour daylight</t>
+  </si>
+  <si>
+    <t>QB transitions in darkness</t>
+  </si>
+  <si>
+    <t>QB transitions per-hour darkness</t>
+  </si>
+  <si>
+    <t>Winter</t>
+  </si>
+  <si>
+    <t>311-35</t>
+  </si>
+  <si>
+    <t>84</t>
+  </si>
+  <si>
+    <t>6.55 ± 0.79</t>
+  </si>
+  <si>
+    <t>19.90 ± 1.13</t>
+  </si>
+  <si>
+    <t>4.07 ± 0.88</t>
+  </si>
+  <si>
+    <t>62% ± 13%</t>
+  </si>
+  <si>
+    <t>15.84 ± 1.03</t>
+  </si>
+  <si>
+    <t>91% ± 6%</t>
+  </si>
+  <si>
+    <t>195 ± 37</t>
+  </si>
+  <si>
+    <t>89 ± 28</t>
+  </si>
+  <si>
+    <t>14 ± 4</t>
+  </si>
+  <si>
+    <t>107 ± 29
+</t>
+  </si>
+  <si>
+    <t>6 ± 2
+</t>
+  </si>
+  <si>
+    <t>Spring</t>
+  </si>
+  <si>
+    <t>36-127</t>
+  </si>
+  <si>
+    <t>88</t>
+  </si>
+  <si>
+    <t>12.44 ± 2.52</t>
+  </si>
+  <si>
+    <t>17.86 ± 2.13</t>
+  </si>
+  <si>
+    <t>6.64 ± 1.95</t>
+  </si>
+  <si>
+    <t>53% ± 16%</t>
+  </si>
+  <si>
+    <t>11.22 ± 2.38</t>
+  </si>
+  <si>
+    <t>97% ± 21%</t>
+  </si>
+  <si>
+    <t>248 ± 47</t>
+  </si>
+  <si>
+    <t>181 ± 50</t>
+  </si>
+  <si>
+    <t>15 ± 4</t>
+  </si>
+  <si>
+    <t>67 ± 28
+</t>
+  </si>
+  <si>
+    <t>6 ± 2
+</t>
+  </si>
+  <si>
+    <t>Summer</t>
+  </si>
+  <si>
+    <t>128-218</t>
+  </si>
+  <si>
+    <t>75</t>
+  </si>
+  <si>
+    <t>18.21 ± 0.81</t>
+  </si>
+  <si>
+    <t>15.40 ± 1.85</t>
+  </si>
+  <si>
+    <t>10.26 ± 1.96</t>
+  </si>
+  <si>
+    <t>56% ± 11%</t>
+  </si>
+  <si>
+    <t>5.15 ± 0.75</t>
+  </si>
+  <si>
+    <t>89% ± 13%</t>
+  </si>
+  <si>
+    <t>296 ± 45</t>
+  </si>
+  <si>
+    <t>262 ± 41</t>
+  </si>
+  <si>
+    <t>14 ± 2</t>
+  </si>
+  <si>
+    <t>34 ± 16
+</t>
+  </si>
+  <si>
+    <t>6 ± 3
+</t>
+  </si>
+  <si>
+    <t>Autumn</t>
+  </si>
+  <si>
+    <t>219-309</t>
+  </si>
+  <si>
+    <t>98</t>
+  </si>
+  <si>
+    <t>12.37 ± 2.47</t>
+  </si>
+  <si>
+    <t>13.74 ± 2.26</t>
+  </si>
+  <si>
+    <t>4.59 ± 2.34</t>
+  </si>
+  <si>
+    <t>37% ± 19%</t>
+  </si>
+  <si>
+    <t>9.16 ± 1.09</t>
+  </si>
+  <si>
+    <t>79% ± 9%</t>
+  </si>
+  <si>
+    <t>246 ± 55</t>
+  </si>
+  <si>
+    <t>178 ± 45</t>
+  </si>
+  <si>
+    <t>14 ± 4</t>
+  </si>
+  <si>
+    <t>68 ± 23
+</t>
+  </si>
+  <si>
+    <t>6 ± 2
+</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>1-366</t>
+  </si>
+  <si>
+    <t>345</t>
+  </si>
+  <si>
+    <t>12.38 ± 4.52</t>
+  </si>
+  <si>
+    <t>16.96 ± 3.02</t>
+  </si>
+  <si>
+    <t>6.37 ± 3.13</t>
+  </si>
+  <si>
+    <t>51% ± 25%</t>
+  </si>
+  <si>
+    <t>10.58 ± 4.40</t>
+  </si>
+  <si>
+    <t>91% ± 38%</t>
+  </si>
+  <si>
+    <t>244 ± 60</t>
+  </si>
+  <si>
+    <t>173 ± 78</t>
+  </si>
+  <si>
+    <t>14 ± 6</t>
+  </si>
+  <si>
+    <t>71 ± 37</t>
+  </si>
+  <si>
+    <t>6 ± 3
+</t>
+  </si>
+  <si>
+    <t>OriginalVariableNames</t>
+  </si>
+  <si>
+    <t>Julian Day of Year</t>
+  </si>
+  <si>
+    <t>Recording Sessions</t>
+  </si>
+  <si>
+    <t>Unique Squirrels</t>
+  </si>
+  <si>
+    <t>Day Length (hrs)</t>
+  </si>
+  <si>
+    <t>QB per day (hrs)</t>
+  </si>
+  <si>
+    <t>QB in daylight (hrs)</t>
+  </si>
+  <si>
+    <t>QB in daylight (%)</t>
+  </si>
+  <si>
+    <t>QB in darkness (hrs)</t>
+  </si>
+  <si>
+    <t>QB in darkness (%)</t>
+  </si>
+  <si>
+    <t>Total QB transitions</t>
+  </si>
+  <si>
+    <t>QB transitions in daylight</t>
+  </si>
+  <si>
+    <t>QB transitions per-hour daylight</t>
+  </si>
+  <si>
+    <t>QB transitions in darkness</t>
+  </si>
+  <si>
+    <t>QB transitions per-hour darkness</t>
+  </si>
+  <si>
+    <t>Winter</t>
+  </si>
+  <si>
+    <t>311-35</t>
+  </si>
+  <si>
+    <t>84</t>
+  </si>
+  <si>
+    <t>6.55 ± 0.79</t>
+  </si>
+  <si>
+    <t>19.91 ± 1.13</t>
+  </si>
+  <si>
+    <t>4.07 ± 0.88</t>
+  </si>
+  <si>
+    <t>62% ± 13%</t>
+  </si>
+  <si>
+    <t>15.84 ± 1.03</t>
+  </si>
+  <si>
+    <t>91% ± 6%</t>
+  </si>
+  <si>
+    <t>195 ± 37</t>
+  </si>
+  <si>
+    <t>89 ± 28</t>
+  </si>
+  <si>
+    <t>14 ± 4</t>
+  </si>
+  <si>
+    <t>107 ± 29
+</t>
+  </si>
+  <si>
+    <t>6 ± 2
+</t>
+  </si>
+  <si>
+    <t>Spring</t>
+  </si>
+  <si>
+    <t>36-127</t>
+  </si>
+  <si>
+    <t>88</t>
+  </si>
+  <si>
+    <t>12.44 ± 2.52</t>
+  </si>
+  <si>
+    <t>17.92 ± 2.12</t>
+  </si>
+  <si>
+    <t>6.69 ± 1.92</t>
+  </si>
+  <si>
+    <t>54% ± 15%</t>
+  </si>
+  <si>
+    <t>11.23 ± 2.39</t>
+  </si>
+  <si>
+    <t>97% ± 21%</t>
+  </si>
+  <si>
+    <t>249 ± 47</t>
+  </si>
+  <si>
+    <t>183 ± 50</t>
+  </si>
+  <si>
+    <t>15 ± 4</t>
+  </si>
+  <si>
+    <t>66 ± 28
+</t>
+  </si>
+  <si>
+    <t>6 ± 2
+</t>
+  </si>
+  <si>
+    <t>Summer</t>
+  </si>
+  <si>
+    <t>128-218</t>
+  </si>
+  <si>
+    <t>75</t>
+  </si>
+  <si>
+    <t>18.21 ± 0.81</t>
+  </si>
+  <si>
+    <t>15.48 ± 1.81</t>
+  </si>
+  <si>
+    <t>10.33 ± 1.94</t>
+  </si>
+  <si>
+    <t>57% ± 11%</t>
+  </si>
+  <si>
+    <t>5.15 ± 0.75</t>
+  </si>
+  <si>
+    <t>89% ± 13%</t>
+  </si>
+  <si>
+    <t>298 ± 45</t>
+  </si>
+  <si>
+    <t>264 ± 41</t>
+  </si>
+  <si>
+    <t>14 ± 2</t>
+  </si>
+  <si>
+    <t>34 ± 16
+</t>
+  </si>
+  <si>
+    <t>6 ± 3
+</t>
+  </si>
+  <si>
+    <t>Autumn</t>
+  </si>
+  <si>
+    <t>219-309</t>
+  </si>
+  <si>
+    <t>98</t>
+  </si>
+  <si>
+    <t>12.37 ± 2.47</t>
+  </si>
+  <si>
+    <t>13.75 ± 2.26</t>
+  </si>
+  <si>
+    <t>4.59 ± 2.34</t>
+  </si>
+  <si>
+    <t>37% ± 19%</t>
+  </si>
+  <si>
+    <t>9.16 ± 1.09</t>
+  </si>
+  <si>
+    <t>79% ± 9%</t>
+  </si>
+  <si>
+    <t>246 ± 55</t>
+  </si>
+  <si>
+    <t>178 ± 45</t>
+  </si>
+  <si>
+    <t>14 ± 4</t>
+  </si>
+  <si>
+    <t>68 ± 23
+</t>
+  </si>
+  <si>
+    <t>6 ± 2
+</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>1-366</t>
+  </si>
+  <si>
+    <t>345</t>
+  </si>
+  <si>
+    <t>12.38 ± 4.52</t>
+  </si>
+  <si>
+    <t>16.99 ± 3.01</t>
+  </si>
+  <si>
+    <t>6.40 ± 3.14</t>
+  </si>
+  <si>
+    <t>52% ± 25%</t>
+  </si>
+  <si>
+    <t>10.59 ± 4.40</t>
+  </si>
+  <si>
+    <t>91% ± 38%</t>
+  </si>
+  <si>
+    <t>245 ± 60</t>
+  </si>
+  <si>
+    <t>174 ± 79</t>
+  </si>
+  <si>
+    <t>14 ± 6</t>
+  </si>
+  <si>
+    <t>71 ± 37</t>
+  </si>
+  <si>
+    <t>6 ± 3
+</t>
+  </si>
+  <si>
+    <t>OriginalVariableNames</t>
+  </si>
+  <si>
+    <t>Julian Day of Year</t>
+  </si>
+  <si>
+    <t>Recording Sessions</t>
+  </si>
+  <si>
+    <t>Unique Squirrels</t>
+  </si>
+  <si>
+    <t>Day Length (hrs)</t>
+  </si>
+  <si>
+    <t>QB per day (hrs)</t>
+  </si>
+  <si>
+    <t>QB in daylight (hrs)</t>
+  </si>
+  <si>
+    <t>QB in daylight (%)</t>
+  </si>
+  <si>
+    <t>QB in darkness (hrs)</t>
+  </si>
+  <si>
+    <t>QB in darkness (%)</t>
+  </si>
+  <si>
+    <t>Total QB transitions</t>
+  </si>
+  <si>
+    <t>QB transitions in daylight</t>
+  </si>
+  <si>
+    <t>QB transitions per-hour daylight</t>
+  </si>
+  <si>
+    <t>QB transitions in darkness</t>
+  </si>
+  <si>
+    <t>QB transitions per-hour darkness</t>
+  </si>
+  <si>
+    <t>Winter</t>
+  </si>
+  <si>
+    <t>311-35</t>
+  </si>
+  <si>
+    <t>84</t>
+  </si>
+  <si>
+    <t>6.55 ± 0.79</t>
+  </si>
+  <si>
+    <t>19.90 ± 1.13</t>
+  </si>
+  <si>
+    <t>4.07 ± 0.88</t>
+  </si>
+  <si>
+    <t>62% ± 13%</t>
+  </si>
+  <si>
+    <t>15.84 ± 1.03</t>
+  </si>
+  <si>
+    <t>91% ± 6%</t>
+  </si>
+  <si>
+    <t>195 ± 37</t>
+  </si>
+  <si>
+    <t>89 ± 28</t>
+  </si>
+  <si>
+    <t>14 ± 4</t>
+  </si>
+  <si>
+    <t>107 ± 29
+</t>
+  </si>
+  <si>
+    <t>6 ± 2
+</t>
+  </si>
+  <si>
+    <t>Spring</t>
+  </si>
+  <si>
+    <t>36-127</t>
+  </si>
+  <si>
+    <t>88</t>
+  </si>
+  <si>
+    <t>12.44 ± 2.52</t>
+  </si>
+  <si>
+    <t>18.05 ± 2.62</t>
+  </si>
+  <si>
+    <t>6.85 ± 2.02</t>
+  </si>
+  <si>
+    <t>55% ± 16%</t>
+  </si>
+  <si>
+    <t>11.20 ± 2.53</t>
+  </si>
+  <si>
+    <t>97% ± 22%</t>
+  </si>
+  <si>
+    <t>248 ± 55</t>
+  </si>
+  <si>
+    <t>177 ± 57</t>
+  </si>
+  <si>
+    <t>14 ± 5</t>
+  </si>
+  <si>
+    <t>71 ± 30
+</t>
+  </si>
+  <si>
+    <t>6 ± 3
+</t>
+  </si>
+  <si>
+    <t>Summer</t>
+  </si>
+  <si>
+    <t>128-218</t>
+  </si>
+  <si>
+    <t>75</t>
+  </si>
+  <si>
+    <t>18.21 ± 0.81</t>
+  </si>
+  <si>
+    <t>15.56 ± 1.80</t>
+  </si>
+  <si>
+    <t>9.93 ± 1.95</t>
+  </si>
+  <si>
+    <t>55% ± 11%</t>
+  </si>
+  <si>
+    <t>5.63 ± 0.73</t>
+  </si>
+  <si>
+    <t>97% ± 13%</t>
+  </si>
+  <si>
+    <t>294 ± 40</t>
+  </si>
+  <si>
+    <t>262 ± 37</t>
+  </si>
+  <si>
+    <t>14 ± 2</t>
+  </si>
+  <si>
+    <t>32 ± 12
+</t>
+  </si>
+  <si>
+    <t>6 ± 2
+</t>
+  </si>
+  <si>
+    <t>Autumn</t>
+  </si>
+  <si>
+    <t>219-309</t>
+  </si>
+  <si>
+    <t>98</t>
+  </si>
+  <si>
+    <t>12.37 ± 2.47</t>
+  </si>
+  <si>
+    <t>15.01 ± 1.62</t>
+  </si>
+  <si>
+    <t>5.76 ± 1.57</t>
+  </si>
+  <si>
+    <t>47% ± 13%</t>
+  </si>
+  <si>
+    <t>9.24 ± 1.07</t>
+  </si>
+  <si>
+    <t>79% ± 9%</t>
+  </si>
+  <si>
+    <t>244 ± 41</t>
+  </si>
+  <si>
+    <t>183 ± 34</t>
+  </si>
+  <si>
+    <t>15 ± 3</t>
+  </si>
+  <si>
+    <t>61 ± 19
+</t>
+  </si>
+  <si>
+    <t>5 ± 2
+</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>1-366</t>
+  </si>
+  <si>
+    <t>345</t>
+  </si>
+  <si>
+    <t>12.38 ± 4.52</t>
+  </si>
+  <si>
+    <t>18.33 ± 2.59</t>
+  </si>
+  <si>
+    <t>5.30 ± 2.17</t>
+  </si>
+  <si>
+    <t>43% ± 18%</t>
+  </si>
+  <si>
+    <t>13.03 ± 3.69</t>
+  </si>
+  <si>
+    <t>112% ± 32%</t>
+  </si>
+  <si>
+    <t>221 ± 52</t>
+  </si>
+  <si>
+    <t>134 ± 67</t>
+  </si>
+  <si>
+    <t>11 ± 5</t>
+  </si>
+  <si>
+    <t>87 ± 36</t>
+  </si>
+  <si>
+    <t>7 ± 3
+</t>
+  </si>
+  <si>
+    <t>OriginalVariableNames</t>
+  </si>
+  <si>
+    <t>Julian Day of Year</t>
+  </si>
+  <si>
+    <t>Recording Sessions</t>
+  </si>
+  <si>
+    <t>Unique Squirrels</t>
+  </si>
+  <si>
+    <t>Day Length (hrs)</t>
+  </si>
+  <si>
+    <t>QB per day (hrs)</t>
+  </si>
+  <si>
+    <t>QB in daylight (hrs)</t>
+  </si>
+  <si>
+    <t>QB in daylight (%)</t>
+  </si>
+  <si>
+    <t>QB in darkness (hrs)</t>
+  </si>
+  <si>
+    <t>QB in darkness (%)</t>
+  </si>
+  <si>
+    <t>Total QB transitions</t>
+  </si>
+  <si>
+    <t>QB transitions in daylight</t>
+  </si>
+  <si>
+    <t>QB transitions per-hour daylight</t>
+  </si>
+  <si>
+    <t>QB transitions in darkness</t>
+  </si>
+  <si>
+    <t>QB transitions per-hour darkness</t>
+  </si>
+  <si>
+    <t>Winter</t>
+  </si>
+  <si>
+    <t>311-35</t>
+  </si>
+  <si>
+    <t>6.55 ± 0.79</t>
+  </si>
+  <si>
+    <t>19.90 ± 1.13</t>
+  </si>
+  <si>
+    <t>4.07 ± 0.88</t>
+  </si>
+  <si>
+    <t>62% ± 13%</t>
+  </si>
+  <si>
+    <t>15.84 ± 1.03</t>
+  </si>
+  <si>
+    <t>91% ± 6%</t>
+  </si>
+  <si>
+    <t>195 ± 37</t>
+  </si>
+  <si>
+    <t>89 ± 28</t>
+  </si>
+  <si>
+    <t>14 ± 4</t>
+  </si>
+  <si>
+    <t>107 ± 29
+</t>
+  </si>
+  <si>
+    <t>6 ± 2
+</t>
+  </si>
+  <si>
+    <t>Spring</t>
+  </si>
+  <si>
+    <t>36-127</t>
+  </si>
+  <si>
+    <t>12.44 ± 2.52</t>
+  </si>
+  <si>
+    <t>17.86 ± 2.13</t>
+  </si>
+  <si>
+    <t>6.64 ± 1.95</t>
+  </si>
+  <si>
+    <t>53% ± 16%</t>
+  </si>
+  <si>
+    <t>11.22 ± 2.38</t>
+  </si>
+  <si>
+    <t>97% ± 21%</t>
+  </si>
+  <si>
+    <t>248 ± 47</t>
+  </si>
+  <si>
+    <t>181 ± 50</t>
+  </si>
+  <si>
+    <t>15 ± 4</t>
+  </si>
+  <si>
+    <t>67 ± 28
+</t>
+  </si>
+  <si>
+    <t>6 ± 2
+</t>
+  </si>
+  <si>
+    <t>Summer</t>
+  </si>
+  <si>
+    <t>128-218</t>
+  </si>
+  <si>
+    <t>18.21 ± 0.81</t>
+  </si>
+  <si>
+    <t>15.40 ± 1.85</t>
+  </si>
+  <si>
+    <t>10.26 ± 1.96</t>
+  </si>
+  <si>
+    <t>56% ± 11%</t>
+  </si>
+  <si>
+    <t>5.15 ± 0.75</t>
+  </si>
+  <si>
+    <t>89% ± 13%</t>
+  </si>
+  <si>
+    <t>296 ± 45</t>
+  </si>
+  <si>
+    <t>262 ± 41</t>
+  </si>
+  <si>
+    <t>14 ± 2</t>
+  </si>
+  <si>
+    <t>34 ± 16
+</t>
+  </si>
+  <si>
+    <t>6 ± 3
+</t>
+  </si>
+  <si>
+    <t>Autumn</t>
+  </si>
+  <si>
+    <t>219-309</t>
+  </si>
+  <si>
+    <t>12.37 ± 2.47</t>
+  </si>
+  <si>
+    <t>13.74 ± 2.26</t>
+  </si>
+  <si>
+    <t>4.59 ± 2.34</t>
+  </si>
+  <si>
+    <t>37% ± 19%</t>
+  </si>
+  <si>
+    <t>9.16 ± 1.09</t>
+  </si>
+  <si>
+    <t>79% ± 9%</t>
+  </si>
+  <si>
+    <t>246 ± 55</t>
+  </si>
+  <si>
+    <t>178 ± 45</t>
+  </si>
+  <si>
+    <t>14 ± 4</t>
+  </si>
+  <si>
+    <t>68 ± 23
+</t>
+  </si>
+  <si>
+    <t>6 ± 2
+</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>1-366</t>
+  </si>
+  <si>
+    <t>12.39 ± 1.65</t>
+  </si>
+  <si>
+    <t>16.72 ± 1.84</t>
+  </si>
+  <si>
+    <t>6.39 ± 1.78</t>
+  </si>
+  <si>
+    <t>NaN% ± NaN%</t>
+  </si>
+  <si>
+    <t>10.34 ± 1.31</t>
+  </si>
+  <si>
+    <t>NaN% ± NaN%</t>
+  </si>
+  <si>
+    <t>246 ± 46</t>
+  </si>
+  <si>
+    <t>41 ± 178</t>
+  </si>
+  <si>
+    <t>14 ± 4</t>
+  </si>
+  <si>
+    <t>69 ± 24</t>
+  </si>
+  <si>
+    <t>6 ± 2
+</t>
+  </si>
+  <si>
+    <t>OriginalVariableNames</t>
+  </si>
+  <si>
+    <t>Julian Day of Year</t>
+  </si>
+  <si>
+    <t>Recording Sessions</t>
+  </si>
+  <si>
+    <t>Unique Squirrels</t>
+  </si>
+  <si>
+    <t>Day Length (hrs)</t>
+  </si>
+  <si>
+    <t>QB per day (hrs)</t>
+  </si>
+  <si>
+    <t>QB in daylight (hrs)</t>
+  </si>
+  <si>
+    <t>QB in daylight (%)</t>
+  </si>
+  <si>
+    <t>QB in darkness (hrs)</t>
+  </si>
+  <si>
+    <t>QB in darkness (%)</t>
+  </si>
+  <si>
+    <t>Total QB transitions</t>
+  </si>
+  <si>
+    <t>QB transitions in daylight</t>
+  </si>
+  <si>
+    <t>QB transitions per-hour daylight</t>
+  </si>
+  <si>
+    <t>QB transitions in darkness</t>
+  </si>
+  <si>
+    <t>QB transitions per-hour darkness</t>
+  </si>
+  <si>
+    <t>Winter</t>
+  </si>
+  <si>
+    <t>311-35</t>
+  </si>
+  <si>
+    <t>6.55 ± 0.79</t>
+  </si>
+  <si>
+    <t>19.90 ± 1.13</t>
+  </si>
+  <si>
+    <t>4.07 ± 0.88</t>
+  </si>
+  <si>
+    <t>62% ± 13%</t>
+  </si>
+  <si>
+    <t>15.84 ± 1.03</t>
+  </si>
+  <si>
+    <t>91% ± 6%</t>
+  </si>
+  <si>
+    <t>195 ± 37</t>
+  </si>
+  <si>
+    <t>89 ± 28</t>
+  </si>
+  <si>
+    <t>14 ± 4</t>
+  </si>
+  <si>
+    <t>107 ± 29
+</t>
+  </si>
+  <si>
+    <t>6 ± 2
+</t>
+  </si>
+  <si>
+    <t>Spring</t>
+  </si>
+  <si>
+    <t>36-127</t>
+  </si>
+  <si>
+    <t>12.44 ± 2.52</t>
+  </si>
+  <si>
+    <t>17.86 ± 2.13</t>
+  </si>
+  <si>
+    <t>6.64 ± 1.95</t>
+  </si>
+  <si>
+    <t>53% ± 16%</t>
+  </si>
+  <si>
+    <t>11.22 ± 2.38</t>
+  </si>
+  <si>
+    <t>97% ± 21%</t>
+  </si>
+  <si>
+    <t>248 ± 47</t>
+  </si>
+  <si>
+    <t>181 ± 50</t>
+  </si>
+  <si>
+    <t>15 ± 4</t>
+  </si>
+  <si>
+    <t>67 ± 28
+</t>
+  </si>
+  <si>
+    <t>6 ± 2
+</t>
+  </si>
+  <si>
+    <t>Summer</t>
+  </si>
+  <si>
+    <t>128-218</t>
+  </si>
+  <si>
+    <t>18.21 ± 0.81</t>
+  </si>
+  <si>
+    <t>15.40 ± 1.85</t>
+  </si>
+  <si>
+    <t>10.26 ± 1.96</t>
+  </si>
+  <si>
+    <t>56% ± 11%</t>
+  </si>
+  <si>
+    <t>5.15 ± 0.75</t>
+  </si>
+  <si>
+    <t>89% ± 13%</t>
+  </si>
+  <si>
+    <t>296 ± 45</t>
+  </si>
+  <si>
+    <t>262 ± 41</t>
+  </si>
+  <si>
+    <t>14 ± 2</t>
+  </si>
+  <si>
+    <t>34 ± 16
+</t>
+  </si>
+  <si>
+    <t>6 ± 3
+</t>
+  </si>
+  <si>
+    <t>Autumn</t>
+  </si>
+  <si>
+    <t>219-309</t>
+  </si>
+  <si>
+    <t>12.37 ± 2.47</t>
+  </si>
+  <si>
+    <t>13.74 ± 2.26</t>
+  </si>
+  <si>
+    <t>4.59 ± 2.34</t>
+  </si>
+  <si>
+    <t>37% ± 19%</t>
+  </si>
+  <si>
+    <t>9.16 ± 1.09</t>
+  </si>
+  <si>
+    <t>79% ± 9%</t>
+  </si>
+  <si>
+    <t>246 ± 55</t>
+  </si>
+  <si>
+    <t>178 ± 45</t>
+  </si>
+  <si>
+    <t>14 ± 4</t>
+  </si>
+  <si>
+    <t>68 ± 23
+</t>
+  </si>
+  <si>
+    <t>6 ± 2
+</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>1-366</t>
+  </si>
+  <si>
+    <t>12.39 ± 1.65</t>
+  </si>
+  <si>
+    <t>16.72 ± 1.84</t>
+  </si>
+  <si>
+    <t>6.39 ± 1.78</t>
+  </si>
+  <si>
+    <t>15% ± 52%</t>
+  </si>
+  <si>
+    <t>10.34 ± 1.31</t>
+  </si>
+  <si>
+    <t>89% ± 12%</t>
+  </si>
+  <si>
+    <t>246 ± 46</t>
+  </si>
+  <si>
+    <t>41 ± 178</t>
+  </si>
+  <si>
+    <t>14 ± 4</t>
+  </si>
+  <si>
+    <t>69 ± 24</t>
+  </si>
+  <si>
+    <t>6 ± 2
+</t>
   </si>
 </sst>
 </file>
@@ -2696,7 +6098,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -2721,11 +6123,24 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -2744,6 +6159,19 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2753,10 +6181,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F15"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="25.7109375" customWidth="true"/>
+    <col min="1" max="1" width="29.42578125" customWidth="true"/>
     <col min="2" max="2" width="11.140625" customWidth="true"/>
     <col min="3" max="3" width="11.140625" customWidth="true"/>
     <col min="4" max="4" width="11.140625" customWidth="true"/>
@@ -2766,67 +6194,67 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>804</v>
+        <v>1880</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>815</v>
+        <v>1895</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>825</v>
+        <v>1908</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>835</v>
+        <v>1921</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>845</v>
+        <v>1934</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>855</v>
+        <v>1947</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>805</v>
+        <v>1881</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>816</v>
+        <v>1896</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>826</v>
+        <v>1909</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>836</v>
+        <v>1922</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>846</v>
+        <v>1935</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>856</v>
+        <v>1948</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>806</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>817</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>827</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>837</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>847</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>857</v>
+        <v>1882</v>
+      </c>
+      <c r="B3" s="0">
+        <v>84</v>
+      </c>
+      <c r="C3" s="0">
+        <v>88</v>
+      </c>
+      <c r="D3" s="0">
+        <v>75</v>
+      </c>
+      <c r="E3" s="0">
+        <v>98</v>
+      </c>
+      <c r="F3" s="0">
+        <v>345</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>807</v>
+        <v>1883</v>
       </c>
       <c r="B4" s="0">
         <v>71</v>
@@ -2841,147 +6269,227 @@
         <v>68</v>
       </c>
       <c r="F4" s="0">
-        <v>218</v>
+        <v>272</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>808</v>
+        <v>1884</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>818</v>
+        <v>1897</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>828</v>
+        <v>1910</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>838</v>
+        <v>1923</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>848</v>
+        <v>1936</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>858</v>
+        <v>1949</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>809</v>
+        <v>1885</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>819</v>
+        <v>1898</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>829</v>
+        <v>1911</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>839</v>
+        <v>1924</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>849</v>
+        <v>1937</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>859</v>
+        <v>1950</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>810</v>
+        <v>1886</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>820</v>
+        <v>1899</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>830</v>
+        <v>1912</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>840</v>
+        <v>1925</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>850</v>
+        <v>1938</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>860</v>
+        <v>1951</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
-        <v>811</v>
+        <v>1887</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>821</v>
+        <v>1900</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>831</v>
+        <v>1913</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>841</v>
+        <v>1926</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>851</v>
+        <v>1939</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>861</v>
+        <v>1952</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0" t="s">
-        <v>812</v>
+        <v>1888</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>822</v>
+        <v>1901</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>832</v>
+        <v>1914</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>842</v>
+        <v>1927</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>852</v>
+        <v>1940</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>862</v>
+        <v>1953</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
-        <v>813</v>
+        <v>1889</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>823</v>
+        <v>1902</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>833</v>
+        <v>1915</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>843</v>
+        <v>1928</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>853</v>
+        <v>1941</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>863</v>
+        <v>1954</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0" t="s">
-        <v>814</v>
+        <v>1890</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>824</v>
+        <v>1903</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>834</v>
+        <v>1916</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>844</v>
+        <v>1929</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>854</v>
+        <v>1942</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>864</v>
+        <v>1955</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="s">
+        <v>1891</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>1904</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>1917</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>1930</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>1943</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>1956</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="s">
+        <v>1892</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>1905</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>1918</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>1931</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>1944</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>1957</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="s">
+        <v>1893</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>1906</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>1919</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>1932</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>1945</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>1958</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="s">
+        <v>1894</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>1907</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>1920</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>1933</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>1946</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>1959</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
using heatmaps for transition data
</commit_message>
<xml_diff>
--- a/Tstats.xlsx
+++ b/Tstats.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1960" uniqueCount="1960">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2280" uniqueCount="2276">
   <si>
     <t>OriginalVariableNames</t>
   </si>
@@ -6068,6 +6068,989 @@
   </si>
   <si>
     <t>41 ± 178</t>
+  </si>
+  <si>
+    <t>14 ± 4</t>
+  </si>
+  <si>
+    <t>69 ± 24</t>
+  </si>
+  <si>
+    <t>6 ± 2
+</t>
+  </si>
+  <si>
+    <t>OriginalVariableNames</t>
+  </si>
+  <si>
+    <t>Julian Day of Year</t>
+  </si>
+  <si>
+    <t>Recording Sessions</t>
+  </si>
+  <si>
+    <t>Unique Squirrels</t>
+  </si>
+  <si>
+    <t>Day Length (hrs)</t>
+  </si>
+  <si>
+    <t>QB per day (hrs)</t>
+  </si>
+  <si>
+    <t>QB in daylight (hrs)</t>
+  </si>
+  <si>
+    <t>QB in daylight (%)</t>
+  </si>
+  <si>
+    <t>QB in darkness (hrs)</t>
+  </si>
+  <si>
+    <t>QB in darkness (%)</t>
+  </si>
+  <si>
+    <t>Total QB transitions</t>
+  </si>
+  <si>
+    <t>QB transitions in daylight</t>
+  </si>
+  <si>
+    <t>QB transitions per-hour daylight</t>
+  </si>
+  <si>
+    <t>QB transitions in darkness</t>
+  </si>
+  <si>
+    <t>QB transitions per-hour darkness</t>
+  </si>
+  <si>
+    <t>Winter</t>
+  </si>
+  <si>
+    <t>311-35</t>
+  </si>
+  <si>
+    <t>6.55 ± 0.79</t>
+  </si>
+  <si>
+    <t>19.90 ± 1.13</t>
+  </si>
+  <si>
+    <t>4.07 ± 0.88</t>
+  </si>
+  <si>
+    <t>62% ± 13%</t>
+  </si>
+  <si>
+    <t>15.84 ± 1.03</t>
+  </si>
+  <si>
+    <t>91% ± 6%</t>
+  </si>
+  <si>
+    <t>195 ± 37</t>
+  </si>
+  <si>
+    <t>89 ± 28</t>
+  </si>
+  <si>
+    <t>14 ± 4</t>
+  </si>
+  <si>
+    <t>107 ± 29
+</t>
+  </si>
+  <si>
+    <t>6 ± 2
+</t>
+  </si>
+  <si>
+    <t>Spring</t>
+  </si>
+  <si>
+    <t>36-127</t>
+  </si>
+  <si>
+    <t>12.44 ± 2.52</t>
+  </si>
+  <si>
+    <t>17.86 ± 2.13</t>
+  </si>
+  <si>
+    <t>6.64 ± 1.95</t>
+  </si>
+  <si>
+    <t>53% ± 16%</t>
+  </si>
+  <si>
+    <t>11.22 ± 2.38</t>
+  </si>
+  <si>
+    <t>97% ± 21%</t>
+  </si>
+  <si>
+    <t>248 ± 47</t>
+  </si>
+  <si>
+    <t>181 ± 50</t>
+  </si>
+  <si>
+    <t>15 ± 4</t>
+  </si>
+  <si>
+    <t>67 ± 28
+</t>
+  </si>
+  <si>
+    <t>6 ± 2
+</t>
+  </si>
+  <si>
+    <t>Summer</t>
+  </si>
+  <si>
+    <t>128-218</t>
+  </si>
+  <si>
+    <t>18.21 ± 0.81</t>
+  </si>
+  <si>
+    <t>15.40 ± 1.85</t>
+  </si>
+  <si>
+    <t>10.26 ± 1.96</t>
+  </si>
+  <si>
+    <t>56% ± 11%</t>
+  </si>
+  <si>
+    <t>5.15 ± 0.75</t>
+  </si>
+  <si>
+    <t>89% ± 13%</t>
+  </si>
+  <si>
+    <t>296 ± 45</t>
+  </si>
+  <si>
+    <t>262 ± 41</t>
+  </si>
+  <si>
+    <t>14 ± 2</t>
+  </si>
+  <si>
+    <t>34 ± 16
+</t>
+  </si>
+  <si>
+    <t>6 ± 3
+</t>
+  </si>
+  <si>
+    <t>Autumn</t>
+  </si>
+  <si>
+    <t>219-309</t>
+  </si>
+  <si>
+    <t>12.37 ± 2.47</t>
+  </si>
+  <si>
+    <t>13.74 ± 2.26</t>
+  </si>
+  <si>
+    <t>4.59 ± 2.34</t>
+  </si>
+  <si>
+    <t>37% ± 19%</t>
+  </si>
+  <si>
+    <t>9.16 ± 1.09</t>
+  </si>
+  <si>
+    <t>79% ± 9%</t>
+  </si>
+  <si>
+    <t>246 ± 55</t>
+  </si>
+  <si>
+    <t>178 ± 45</t>
+  </si>
+  <si>
+    <t>14 ± 4</t>
+  </si>
+  <si>
+    <t>68 ± 23
+</t>
+  </si>
+  <si>
+    <t>6 ± 2
+</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>1-366</t>
+  </si>
+  <si>
+    <t>12.39 ± 1.65</t>
+  </si>
+  <si>
+    <t>16.72 ± 1.84</t>
+  </si>
+  <si>
+    <t>6.39 ± 1.78</t>
+  </si>
+  <si>
+    <t>15% ± 52%</t>
+  </si>
+  <si>
+    <t>10.34 ± 1.31</t>
+  </si>
+  <si>
+    <t>89% ± 12%</t>
+  </si>
+  <si>
+    <t>246 ± 46</t>
+  </si>
+  <si>
+    <t>41 ± 178</t>
+  </si>
+  <si>
+    <t>14 ± 4</t>
+  </si>
+  <si>
+    <t>69 ± 24</t>
+  </si>
+  <si>
+    <t>6 ± 2
+</t>
+  </si>
+  <si>
+    <t>OriginalVariableNames</t>
+  </si>
+  <si>
+    <t>Julian Day of Year</t>
+  </si>
+  <si>
+    <t>Recording Sessions</t>
+  </si>
+  <si>
+    <t>Unique Squirrels</t>
+  </si>
+  <si>
+    <t>Day Length (hrs)</t>
+  </si>
+  <si>
+    <t>QB per day (hrs)</t>
+  </si>
+  <si>
+    <t>QB in daylight (hrs)</t>
+  </si>
+  <si>
+    <t>QB in daylight (%)</t>
+  </si>
+  <si>
+    <t>QB in darkness (hrs)</t>
+  </si>
+  <si>
+    <t>QB in darkness (%)</t>
+  </si>
+  <si>
+    <t>Total QB transitions</t>
+  </si>
+  <si>
+    <t>QB transitions in daylight</t>
+  </si>
+  <si>
+    <t>QB transitions per-hour daylight</t>
+  </si>
+  <si>
+    <t>QB transitions in darkness</t>
+  </si>
+  <si>
+    <t>QB transitions per-hour darkness</t>
+  </si>
+  <si>
+    <t>Winter</t>
+  </si>
+  <si>
+    <t>311-35</t>
+  </si>
+  <si>
+    <t>6.55 ± 0.79</t>
+  </si>
+  <si>
+    <t>19.90 ± 1.13</t>
+  </si>
+  <si>
+    <t>4.07 ± 0.88</t>
+  </si>
+  <si>
+    <t>62% ± 13%</t>
+  </si>
+  <si>
+    <t>15.84 ± 1.03</t>
+  </si>
+  <si>
+    <t>91% ± 6%</t>
+  </si>
+  <si>
+    <t>195 ± 37</t>
+  </si>
+  <si>
+    <t>89 ± 28</t>
+  </si>
+  <si>
+    <t>14 ± 4</t>
+  </si>
+  <si>
+    <t>107 ± 29
+</t>
+  </si>
+  <si>
+    <t>6 ± 2
+</t>
+  </si>
+  <si>
+    <t>Spring</t>
+  </si>
+  <si>
+    <t>36-127</t>
+  </si>
+  <si>
+    <t>12.44 ± 2.52</t>
+  </si>
+  <si>
+    <t>17.86 ± 2.13</t>
+  </si>
+  <si>
+    <t>6.64 ± 1.95</t>
+  </si>
+  <si>
+    <t>53% ± 16%</t>
+  </si>
+  <si>
+    <t>11.22 ± 2.38</t>
+  </si>
+  <si>
+    <t>97% ± 21%</t>
+  </si>
+  <si>
+    <t>248 ± 47</t>
+  </si>
+  <si>
+    <t>181 ± 50</t>
+  </si>
+  <si>
+    <t>15 ± 4</t>
+  </si>
+  <si>
+    <t>67 ± 28
+</t>
+  </si>
+  <si>
+    <t>6 ± 2
+</t>
+  </si>
+  <si>
+    <t>Summer</t>
+  </si>
+  <si>
+    <t>128-218</t>
+  </si>
+  <si>
+    <t>18.21 ± 0.81</t>
+  </si>
+  <si>
+    <t>15.40 ± 1.85</t>
+  </si>
+  <si>
+    <t>10.26 ± 1.96</t>
+  </si>
+  <si>
+    <t>56% ± 11%</t>
+  </si>
+  <si>
+    <t>5.15 ± 0.75</t>
+  </si>
+  <si>
+    <t>89% ± 13%</t>
+  </si>
+  <si>
+    <t>296 ± 45</t>
+  </si>
+  <si>
+    <t>262 ± 41</t>
+  </si>
+  <si>
+    <t>14 ± 2</t>
+  </si>
+  <si>
+    <t>34 ± 16
+</t>
+  </si>
+  <si>
+    <t>6 ± 3
+</t>
+  </si>
+  <si>
+    <t>Autumn</t>
+  </si>
+  <si>
+    <t>219-309</t>
+  </si>
+  <si>
+    <t>12.37 ± 2.47</t>
+  </si>
+  <si>
+    <t>13.74 ± 2.26</t>
+  </si>
+  <si>
+    <t>4.59 ± 2.34</t>
+  </si>
+  <si>
+    <t>37% ± 19%</t>
+  </si>
+  <si>
+    <t>9.16 ± 1.09</t>
+  </si>
+  <si>
+    <t>79% ± 9%</t>
+  </si>
+  <si>
+    <t>246 ± 55</t>
+  </si>
+  <si>
+    <t>178 ± 45</t>
+  </si>
+  <si>
+    <t>14 ± 4</t>
+  </si>
+  <si>
+    <t>68 ± 23
+</t>
+  </si>
+  <si>
+    <t>6 ± 2
+</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>1-366</t>
+  </si>
+  <si>
+    <t>12.39 ± 1.65</t>
+  </si>
+  <si>
+    <t>16.72 ± 1.84</t>
+  </si>
+  <si>
+    <t>6.39 ± 1.78</t>
+  </si>
+  <si>
+    <t>15% ± 52%</t>
+  </si>
+  <si>
+    <t>10.34 ± 1.31</t>
+  </si>
+  <si>
+    <t>89% ± 12%</t>
+  </si>
+  <si>
+    <t>246 ± 46</t>
+  </si>
+  <si>
+    <t>41 ± 178</t>
+  </si>
+  <si>
+    <t>14 ± 4</t>
+  </si>
+  <si>
+    <t>69 ± 24</t>
+  </si>
+  <si>
+    <t>6 ± 2
+</t>
+  </si>
+  <si>
+    <t>OriginalVariableNames</t>
+  </si>
+  <si>
+    <t>Julian Day of Year</t>
+  </si>
+  <si>
+    <t>Recording Sessions</t>
+  </si>
+  <si>
+    <t>Unique Squirrels</t>
+  </si>
+  <si>
+    <t>Day Length (hrs)</t>
+  </si>
+  <si>
+    <t>QB per day (hrs)</t>
+  </si>
+  <si>
+    <t>QB in daylight (hrs)</t>
+  </si>
+  <si>
+    <t>QB in daylight (%)</t>
+  </si>
+  <si>
+    <t>QB in darkness (hrs)</t>
+  </si>
+  <si>
+    <t>QB in darkness (%)</t>
+  </si>
+  <si>
+    <t>Total QB transitions</t>
+  </si>
+  <si>
+    <t>QB transitions in daylight</t>
+  </si>
+  <si>
+    <t>QB transitions per-hour daylight</t>
+  </si>
+  <si>
+    <t>QB transitions in darkness</t>
+  </si>
+  <si>
+    <t>QB transitions per-hour darkness</t>
+  </si>
+  <si>
+    <t>Winter</t>
+  </si>
+  <si>
+    <t>311-35</t>
+  </si>
+  <si>
+    <t>6.55 ± 0.79</t>
+  </si>
+  <si>
+    <t>NaN ± NaN</t>
+  </si>
+  <si>
+    <t>NaN% ± NaN%</t>
+  </si>
+  <si>
+    <t>NaN ± NaN</t>
+  </si>
+  <si>
+    <t>NaN% ± NaN%</t>
+  </si>
+  <si>
+    <t>NaN ± NaN</t>
+  </si>
+  <si>
+    <t>NaN ± NaN
+</t>
+  </si>
+  <si>
+    <t>Spring</t>
+  </si>
+  <si>
+    <t>36-127</t>
+  </si>
+  <si>
+    <t>12.44 ± 2.52</t>
+  </si>
+  <si>
+    <t>17.65 ± 1.35</t>
+  </si>
+  <si>
+    <t>6.41 ± 1.84</t>
+  </si>
+  <si>
+    <t>52% ± 15%</t>
+  </si>
+  <si>
+    <t>11.24 ± 2.21</t>
+  </si>
+  <si>
+    <t>97% ± 19%</t>
+  </si>
+  <si>
+    <t>247 ± 35</t>
+  </si>
+  <si>
+    <t>186 ± 40</t>
+  </si>
+  <si>
+    <t>15 ± 3</t>
+  </si>
+  <si>
+    <t>61 ± 23
+</t>
+  </si>
+  <si>
+    <t>5 ± 2
+</t>
+  </si>
+  <si>
+    <t>Summer</t>
+  </si>
+  <si>
+    <t>128-218</t>
+  </si>
+  <si>
+    <t>18.21 ± 0.81</t>
+  </si>
+  <si>
+    <t>15.38 ± 1.85</t>
+  </si>
+  <si>
+    <t>10.31 ± 1.96</t>
+  </si>
+  <si>
+    <t>57% ± 11%</t>
+  </si>
+  <si>
+    <t>5.06 ± 0.73</t>
+  </si>
+  <si>
+    <t>87% ± 13%</t>
+  </si>
+  <si>
+    <t>296 ± 46</t>
+  </si>
+  <si>
+    <t>262 ± 41</t>
+  </si>
+  <si>
+    <t>14 ± 2</t>
+  </si>
+  <si>
+    <t>35 ± 16
+</t>
+  </si>
+  <si>
+    <t>6 ± 3
+</t>
+  </si>
+  <si>
+    <t>Autumn</t>
+  </si>
+  <si>
+    <t>219-309</t>
+  </si>
+  <si>
+    <t>12.37 ± 2.47</t>
+  </si>
+  <si>
+    <t>12.39 ± 2.07</t>
+  </si>
+  <si>
+    <t>3.33 ± 2.37</t>
+  </si>
+  <si>
+    <t>27% ± 19%</t>
+  </si>
+  <si>
+    <t>9.06 ± 1.11</t>
+  </si>
+  <si>
+    <t>78% ± 10%</t>
+  </si>
+  <si>
+    <t>248 ± 67</t>
+  </si>
+  <si>
+    <t>173 ± 54</t>
+  </si>
+  <si>
+    <t>14 ± 4</t>
+  </si>
+  <si>
+    <t>75 ± 24
+</t>
+  </si>
+  <si>
+    <t>6 ± 2
+</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>1-366</t>
+  </si>
+  <si>
+    <t>12.39 ± 1.65</t>
+  </si>
+  <si>
+    <t>15.14 ± 1.76</t>
+  </si>
+  <si>
+    <t>6.68 ± 2.06</t>
+  </si>
+  <si>
+    <t>45% ± 15%</t>
+  </si>
+  <si>
+    <t>8.45 ± 1.35</t>
+  </si>
+  <si>
+    <t>87% ± 14%</t>
+  </si>
+  <si>
+    <t>264 ± 49</t>
+  </si>
+  <si>
+    <t>207 ± 45</t>
+  </si>
+  <si>
+    <t>14 ± 3</t>
+  </si>
+  <si>
+    <t>57 ± 21</t>
+  </si>
+  <si>
+    <t>6 ± 2
+</t>
+  </si>
+  <si>
+    <t>OriginalVariableNames</t>
+  </si>
+  <si>
+    <t>Julian Day of Year</t>
+  </si>
+  <si>
+    <t>Recording Sessions</t>
+  </si>
+  <si>
+    <t>Unique Squirrels</t>
+  </si>
+  <si>
+    <t>Day Length (hrs)</t>
+  </si>
+  <si>
+    <t>QB per day (hrs)</t>
+  </si>
+  <si>
+    <t>QB in daylight (hrs)</t>
+  </si>
+  <si>
+    <t>QB in daylight (%)</t>
+  </si>
+  <si>
+    <t>QB in darkness (hrs)</t>
+  </si>
+  <si>
+    <t>QB in darkness (%)</t>
+  </si>
+  <si>
+    <t>Total QB transitions</t>
+  </si>
+  <si>
+    <t>QB transitions in daylight</t>
+  </si>
+  <si>
+    <t>QB transitions per-hour daylight</t>
+  </si>
+  <si>
+    <t>QB transitions in darkness</t>
+  </si>
+  <si>
+    <t>QB transitions per-hour darkness</t>
+  </si>
+  <si>
+    <t>Winter</t>
+  </si>
+  <si>
+    <t>311-35</t>
+  </si>
+  <si>
+    <t>6.55 ± 0.79</t>
+  </si>
+  <si>
+    <t>19.90 ± 1.13</t>
+  </si>
+  <si>
+    <t>4.07 ± 0.88</t>
+  </si>
+  <si>
+    <t>62% ± 13%</t>
+  </si>
+  <si>
+    <t>15.84 ± 1.03</t>
+  </si>
+  <si>
+    <t>91% ± 6%</t>
+  </si>
+  <si>
+    <t>195 ± 37</t>
+  </si>
+  <si>
+    <t>89 ± 28</t>
+  </si>
+  <si>
+    <t>14 ± 4</t>
+  </si>
+  <si>
+    <t>107 ± 29
+</t>
+  </si>
+  <si>
+    <t>6 ± 2
+</t>
+  </si>
+  <si>
+    <t>Spring</t>
+  </si>
+  <si>
+    <t>36-127</t>
+  </si>
+  <si>
+    <t>12.44 ± 2.52</t>
+  </si>
+  <si>
+    <t>17.86 ± 2.13</t>
+  </si>
+  <si>
+    <t>6.64 ± 1.95</t>
+  </si>
+  <si>
+    <t>53% ± 16%</t>
+  </si>
+  <si>
+    <t>11.22 ± 2.38</t>
+  </si>
+  <si>
+    <t>97% ± 21%</t>
+  </si>
+  <si>
+    <t>248 ± 47</t>
+  </si>
+  <si>
+    <t>181 ± 50</t>
+  </si>
+  <si>
+    <t>15 ± 4</t>
+  </si>
+  <si>
+    <t>67 ± 28
+</t>
+  </si>
+  <si>
+    <t>6 ± 2
+</t>
+  </si>
+  <si>
+    <t>Summer</t>
+  </si>
+  <si>
+    <t>128-218</t>
+  </si>
+  <si>
+    <t>18.21 ± 0.81</t>
+  </si>
+  <si>
+    <t>15.40 ± 1.85</t>
+  </si>
+  <si>
+    <t>10.26 ± 1.96</t>
+  </si>
+  <si>
+    <t>56% ± 11%</t>
+  </si>
+  <si>
+    <t>5.15 ± 0.75</t>
+  </si>
+  <si>
+    <t>89% ± 13%</t>
+  </si>
+  <si>
+    <t>296 ± 45</t>
+  </si>
+  <si>
+    <t>262 ± 41</t>
+  </si>
+  <si>
+    <t>14 ± 2</t>
+  </si>
+  <si>
+    <t>34 ± 16
+</t>
+  </si>
+  <si>
+    <t>6 ± 3
+</t>
+  </si>
+  <si>
+    <t>Autumn</t>
+  </si>
+  <si>
+    <t>219-309</t>
+  </si>
+  <si>
+    <t>12.37 ± 2.47</t>
+  </si>
+  <si>
+    <t>13.74 ± 2.26</t>
+  </si>
+  <si>
+    <t>4.59 ± 2.34</t>
+  </si>
+  <si>
+    <t>37% ± 19%</t>
+  </si>
+  <si>
+    <t>9.16 ± 1.09</t>
+  </si>
+  <si>
+    <t>79% ± 9%</t>
+  </si>
+  <si>
+    <t>246 ± 55</t>
+  </si>
+  <si>
+    <t>178 ± 45</t>
+  </si>
+  <si>
+    <t>14 ± 4</t>
+  </si>
+  <si>
+    <t>68 ± 23
+</t>
+  </si>
+  <si>
+    <t>6 ± 2
+</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>1-366</t>
+  </si>
+  <si>
+    <t>12.39 ± 1.65</t>
+  </si>
+  <si>
+    <t>16.72 ± 1.84</t>
+  </si>
+  <si>
+    <t>6.39 ± 1.78</t>
+  </si>
+  <si>
+    <t>52% ± 15%</t>
+  </si>
+  <si>
+    <t>10.34 ± 1.31</t>
+  </si>
+  <si>
+    <t>89% ± 12%</t>
+  </si>
+  <si>
+    <t>246 ± 46</t>
+  </si>
+  <si>
+    <t>178 ± 41</t>
   </si>
   <si>
     <t>14 ± 4</t>
@@ -6098,7 +7081,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="31">
+  <borders count="35">
     <border>
       <left/>
       <right/>
@@ -6136,11 +7119,15 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -6172,6 +7159,10 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6194,47 +7185,47 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>1880</v>
+        <v>2196</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>1895</v>
+        <v>2211</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>1908</v>
+        <v>2224</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>1921</v>
+        <v>2237</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>1934</v>
+        <v>2250</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>1947</v>
+        <v>2263</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>1881</v>
+        <v>2197</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>1896</v>
+        <v>2212</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>1909</v>
+        <v>2225</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>1922</v>
+        <v>2238</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>1935</v>
+        <v>2251</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>1948</v>
+        <v>2264</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>1882</v>
+        <v>2198</v>
       </c>
       <c r="B3" s="0">
         <v>84</v>
@@ -6254,7 +7245,7 @@
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>1883</v>
+        <v>2199</v>
       </c>
       <c r="B4" s="0">
         <v>71</v>
@@ -6274,222 +7265,222 @@
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>1884</v>
+        <v>2200</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>1897</v>
+        <v>2213</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>1910</v>
+        <v>2226</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>1923</v>
+        <v>2239</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>1936</v>
+        <v>2252</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>1949</v>
+        <v>2265</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>1885</v>
+        <v>2201</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>1898</v>
+        <v>2214</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>1911</v>
+        <v>2227</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>1924</v>
+        <v>2240</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>1937</v>
+        <v>2253</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>1950</v>
+        <v>2266</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>1886</v>
+        <v>2202</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>1899</v>
+        <v>2215</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>1912</v>
+        <v>2228</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>1925</v>
+        <v>2241</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>1938</v>
+        <v>2254</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>1951</v>
+        <v>2267</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
-        <v>1887</v>
+        <v>2203</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>1900</v>
+        <v>2216</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>1913</v>
+        <v>2229</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>1926</v>
+        <v>2242</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>1939</v>
+        <v>2255</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>1952</v>
+        <v>2268</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0" t="s">
-        <v>1888</v>
+        <v>2204</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>1901</v>
+        <v>2217</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>1914</v>
+        <v>2230</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>1927</v>
+        <v>2243</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>1940</v>
+        <v>2256</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>1953</v>
+        <v>2269</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
-        <v>1889</v>
+        <v>2205</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>1902</v>
+        <v>2218</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>1915</v>
+        <v>2231</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>1928</v>
+        <v>2244</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>1941</v>
+        <v>2257</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>1954</v>
+        <v>2270</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0" t="s">
-        <v>1890</v>
+        <v>2206</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>1903</v>
+        <v>2219</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>1916</v>
+        <v>2232</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>1929</v>
+        <v>2245</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>1942</v>
+        <v>2258</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>1955</v>
+        <v>2271</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0" t="s">
-        <v>1891</v>
+        <v>2207</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>1904</v>
+        <v>2220</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>1917</v>
+        <v>2233</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>1930</v>
+        <v>2246</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>1943</v>
+        <v>2259</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>1956</v>
+        <v>2272</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0" t="s">
-        <v>1892</v>
+        <v>2208</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>1905</v>
+        <v>2221</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>1918</v>
+        <v>2234</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>1931</v>
+        <v>2247</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>1944</v>
+        <v>2260</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>1957</v>
+        <v>2273</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0" t="s">
-        <v>1893</v>
+        <v>2209</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>1906</v>
+        <v>2222</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>1919</v>
+        <v>2235</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>1932</v>
+        <v>2248</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>1945</v>
+        <v>2261</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>1958</v>
+        <v>2274</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0" t="s">
-        <v>1894</v>
+        <v>2210</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>1907</v>
+        <v>2223</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>1920</v>
+        <v>2236</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>1933</v>
+        <v>2249</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>1946</v>
+        <v>2262</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>1959</v>
+        <v>2275</v>
       </c>
     </row>
   </sheetData>

</xml_diff>